<commit_message>
Complete layout and create NP Gerbers for quote
</commit_message>
<xml_diff>
--- a/Manufacturing/BOM Core 64 v0.4.0 CB Yellow LB Blue.xlsx
+++ b/Manufacturing/BOM Core 64 v0.4.0 CB Yellow LB Blue.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Manufacturing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7537F7-CCD1-F649-885C-59F58EBCA8E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB30509-E052-9345-ABC2-B8DEFA4A074E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="34660" windowHeight="22680" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="34660" windowHeight="22680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SKU List" sheetId="6" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Concept Estimate" sheetId="1" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Core Board V0.4'!$A$6:$N$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Core Board V0.4'!$A$6:$N$73</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'User Supplied Options'!$A$6:$N$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1172" uniqueCount="724">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="731">
   <si>
     <t>Digi-Key Part Number</t>
   </si>
@@ -2226,6 +2226,27 @@
   </si>
   <si>
     <t>4x AAA Battery Holder with keystone connector</t>
+  </si>
+  <si>
+    <t>CORE64-CB-V0.4-NP-1TP-KIT INCLUDED - PRE-ASSEMBLED</t>
+  </si>
+  <si>
+    <t>CM1</t>
+  </si>
+  <si>
+    <t>Header 1x16</t>
+  </si>
+  <si>
+    <t>Header 2x3</t>
+  </si>
+  <si>
+    <t>Core Memory</t>
+  </si>
+  <si>
+    <t>J1, J2</t>
+  </si>
+  <si>
+    <t>do not insert</t>
   </si>
 </sst>
 </file>
@@ -2237,10 +2258,17 @@
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -2498,37 +2526,37 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="17" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="16" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="15" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2538,196 +2566,341 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="14" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="4" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="4" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="4" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2735,197 +2908,68 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="4" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="4" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="4" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="4" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="4" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -3376,10 +3420,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F5DBFB5-E21A-7B4B-815F-748A526FD280}">
-  <dimension ref="A1:R54"/>
+  <dimension ref="A1:R68"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
@@ -3422,11 +3466,11 @@
         <v>172</v>
       </c>
       <c r="C3" s="27"/>
-      <c r="P3" s="154" t="s">
+      <c r="P3" s="161" t="s">
         <v>173</v>
       </c>
-      <c r="Q3" s="154"/>
-      <c r="R3" s="154"/>
+      <c r="Q3" s="161"/>
+      <c r="R3" s="161"/>
     </row>
     <row r="4" spans="1:18" ht="51" x14ac:dyDescent="0.15">
       <c r="A4" s="29"/>
@@ -3533,428 +3577,434 @@
     </row>
     <row r="7" spans="1:18" s="38" customFormat="1" ht="24" x14ac:dyDescent="0.15">
       <c r="A7" s="104" t="s">
-        <v>432</v>
+        <v>724</v>
       </c>
       <c r="B7" s="105"/>
       <c r="C7" s="105"/>
       <c r="D7" s="105"/>
       <c r="R7" s="39"/>
     </row>
-    <row r="8" spans="1:18" ht="17" x14ac:dyDescent="0.15">
-      <c r="A8" s="28">
-        <v>0</v>
-      </c>
-      <c r="B8" s="46" t="s">
-        <v>142</v>
-      </c>
-      <c r="C8" s="56" t="s">
-        <v>352</v>
-      </c>
-      <c r="D8" s="56" t="s">
-        <v>349</v>
-      </c>
-      <c r="E8" s="46">
-        <v>1</v>
-      </c>
-      <c r="F8" s="46" t="s">
+    <row r="8" spans="1:18" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A8" s="60">
+        <v>1</v>
+      </c>
+      <c r="B8" s="165" t="s">
+        <v>321</v>
+      </c>
+      <c r="C8" s="165" t="s">
+        <v>353</v>
+      </c>
+      <c r="D8" s="60" t="s">
+        <v>313</v>
+      </c>
+      <c r="E8" s="166">
+        <v>4</v>
+      </c>
+      <c r="F8" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G8" s="46" t="s">
-        <v>142</v>
-      </c>
-      <c r="H8" s="46" t="s">
-        <v>220</v>
-      </c>
-      <c r="I8" s="46" t="s">
+      <c r="G8" s="38" t="s">
+        <v>201</v>
+      </c>
+      <c r="H8" s="60" t="s">
+        <v>202</v>
+      </c>
+      <c r="I8" s="38" t="s">
         <v>203</v>
       </c>
-      <c r="J8" s="28">
-        <v>0</v>
-      </c>
-      <c r="K8" s="46">
+      <c r="J8" s="38">
+        <v>0</v>
+      </c>
+      <c r="K8" s="38">
+        <f t="shared" ref="K8:K18" si="0">IF(J8&gt;E8,0,E8-J8)</f>
+        <v>4</v>
+      </c>
+      <c r="L8" s="38">
         <v>10</v>
       </c>
-      <c r="M8" s="28">
-        <f>L8-E8</f>
-        <v>-1</v>
-      </c>
-      <c r="N8" s="28">
-        <f>(4*E8)-M8</f>
+      <c r="M8" s="38">
+        <f t="shared" ref="M8:M13" si="1">L8-E8</f>
+        <v>6</v>
+      </c>
+      <c r="N8" s="38">
+        <f t="shared" ref="N8:N13" si="2">(4*E8)-M8</f>
+        <v>10</v>
+      </c>
+      <c r="R8" s="39" t="e">
+        <f t="shared" ref="R8:R14" si="3">Q8/P8</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A9" s="38">
+        <v>2</v>
+      </c>
+      <c r="B9" s="167" t="s">
+        <v>311</v>
+      </c>
+      <c r="C9" s="167" t="s">
+        <v>353</v>
+      </c>
+      <c r="D9" s="60" t="s">
+        <v>313</v>
+      </c>
+      <c r="E9" s="38">
+        <v>1</v>
+      </c>
+      <c r="F9" s="38" t="s">
+        <v>200</v>
+      </c>
+      <c r="G9" s="60" t="s">
+        <v>307</v>
+      </c>
+      <c r="H9" s="60" t="s">
+        <v>337</v>
+      </c>
+      <c r="I9" s="38" t="s">
+        <v>203</v>
+      </c>
+      <c r="J9" s="38">
+        <v>0</v>
+      </c>
+      <c r="K9" s="38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L9" s="38">
+        <v>1</v>
+      </c>
+      <c r="M9" s="38">
+        <f>L9-E9</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="38">
+        <f>(4*E9)-M9</f>
+        <v>4</v>
+      </c>
+      <c r="R9" s="39" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A10" s="38">
+        <v>3</v>
+      </c>
+      <c r="B10" s="60" t="s">
+        <v>221</v>
+      </c>
+      <c r="C10" s="57" t="s">
+        <v>354</v>
+      </c>
+      <c r="D10" s="38" t="s">
+        <v>319</v>
+      </c>
+      <c r="E10" s="38">
+        <v>1</v>
+      </c>
+      <c r="F10" s="38" t="s">
+        <v>200</v>
+      </c>
+      <c r="G10" s="59" t="s">
+        <v>224</v>
+      </c>
+      <c r="H10" s="38" t="s">
+        <v>332</v>
+      </c>
+      <c r="I10" s="60" t="s">
+        <v>203</v>
+      </c>
+      <c r="J10" s="38">
+        <v>0</v>
+      </c>
+      <c r="K10" s="38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L10" s="38">
+        <v>1</v>
+      </c>
+      <c r="M10" s="38">
+        <f t="shared" ref="M10:M15" si="4">L10-E10</f>
+        <v>0</v>
+      </c>
+      <c r="N10" s="38">
+        <f t="shared" ref="N10:N15" si="5">(4*E10)-M10</f>
+        <v>4</v>
+      </c>
+      <c r="R10" s="39" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A11" s="38">
+        <v>4</v>
+      </c>
+      <c r="B11" s="60" t="s">
+        <v>269</v>
+      </c>
+      <c r="C11" s="57" t="s">
+        <v>354</v>
+      </c>
+      <c r="D11" s="38" t="s">
+        <v>319</v>
+      </c>
+      <c r="E11" s="38">
+        <v>1</v>
+      </c>
+      <c r="F11" s="38" t="s">
+        <v>200</v>
+      </c>
+      <c r="G11" s="38" t="s">
+        <v>225</v>
+      </c>
+      <c r="H11" s="60" t="s">
+        <v>333</v>
+      </c>
+      <c r="I11" s="60" t="s">
+        <v>203</v>
+      </c>
+      <c r="J11" s="38">
+        <v>0</v>
+      </c>
+      <c r="K11" s="38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L11" s="38">
+        <v>1</v>
+      </c>
+      <c r="M11" s="38">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="38">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="R11" s="39" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A12" s="38">
         <v>5</v>
       </c>
-      <c r="R8" s="32" t="e">
-        <f t="shared" ref="R8:R15" si="0">Q8/P8</f>
+      <c r="B12" s="60" t="s">
+        <v>222</v>
+      </c>
+      <c r="C12" s="57" t="s">
+        <v>354</v>
+      </c>
+      <c r="D12" s="38" t="s">
+        <v>319</v>
+      </c>
+      <c r="E12" s="38">
+        <v>1</v>
+      </c>
+      <c r="F12" s="38" t="s">
+        <v>200</v>
+      </c>
+      <c r="G12" s="38" t="s">
+        <v>226</v>
+      </c>
+      <c r="H12" s="60" t="s">
+        <v>334</v>
+      </c>
+      <c r="I12" s="60" t="s">
+        <v>203</v>
+      </c>
+      <c r="J12" s="38">
+        <v>0</v>
+      </c>
+      <c r="K12" s="38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L12" s="38">
+        <v>1</v>
+      </c>
+      <c r="M12" s="38">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="38">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="R12" s="39" t="e">
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="17" x14ac:dyDescent="0.15">
-      <c r="A9" s="45">
-        <v>1</v>
-      </c>
-      <c r="B9" s="49" t="s">
-        <v>321</v>
-      </c>
-      <c r="C9" s="49" t="s">
-        <v>353</v>
-      </c>
-      <c r="D9" s="47" t="s">
-        <v>313</v>
-      </c>
-      <c r="E9" s="48">
+    <row r="13" spans="1:18" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A13" s="38">
+        <v>6</v>
+      </c>
+      <c r="B13" s="60" t="s">
+        <v>272</v>
+      </c>
+      <c r="C13" s="57" t="s">
+        <v>354</v>
+      </c>
+      <c r="D13" s="38" t="s">
+        <v>319</v>
+      </c>
+      <c r="E13" s="38">
+        <v>1</v>
+      </c>
+      <c r="F13" s="38" t="s">
+        <v>200</v>
+      </c>
+      <c r="G13" s="38" t="s">
+        <v>227</v>
+      </c>
+      <c r="H13" s="60" t="s">
+        <v>335</v>
+      </c>
+      <c r="I13" s="60" t="s">
+        <v>203</v>
+      </c>
+      <c r="J13" s="38">
+        <v>0</v>
+      </c>
+      <c r="K13" s="38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L13" s="38">
+        <v>1</v>
+      </c>
+      <c r="M13" s="38">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="38">
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="F9" s="46" t="s">
+      <c r="R13" s="39" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" s="38" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="38">
+        <v>7</v>
+      </c>
+      <c r="B14" s="60" t="s">
+        <v>223</v>
+      </c>
+      <c r="C14" s="57" t="s">
+        <v>355</v>
+      </c>
+      <c r="D14" s="59" t="s">
+        <v>340</v>
+      </c>
+      <c r="E14" s="38">
+        <v>1</v>
+      </c>
+      <c r="F14" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G9" s="46" t="s">
-        <v>201</v>
-      </c>
-      <c r="H9" s="47" t="s">
-        <v>202</v>
-      </c>
-      <c r="I9" s="46" t="s">
+      <c r="G14" s="59" t="s">
+        <v>341</v>
+      </c>
+      <c r="H14" s="60" t="s">
+        <v>336</v>
+      </c>
+      <c r="I14" s="60" t="s">
         <v>203</v>
       </c>
-      <c r="J9" s="28">
-        <v>0</v>
-      </c>
-      <c r="K9" s="46">
-        <f t="shared" ref="K9:K18" si="1">IF(J9&gt;E9,0,E9-J9)</f>
+      <c r="J14" s="38">
+        <v>0</v>
+      </c>
+      <c r="K14" s="38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L14" s="38">
+        <v>1</v>
+      </c>
+      <c r="M14" s="38">
+        <f>L14-E14</f>
+        <v>0</v>
+      </c>
+      <c r="N14" s="38">
+        <f>(4*E14)-M14</f>
         <v>4</v>
       </c>
-      <c r="L9" s="38">
-        <v>10</v>
-      </c>
-      <c r="M9" s="28">
-        <f t="shared" ref="M9:M14" si="2">L9-E9</f>
-        <v>6</v>
-      </c>
-      <c r="N9" s="28">
-        <f t="shared" ref="N9:N14" si="3">(4*E9)-M9</f>
-        <v>10</v>
-      </c>
-      <c r="R9" s="32" t="e">
+      <c r="R14" s="39" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" s="35" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="35">
+        <v>8</v>
+      </c>
+      <c r="B15" s="162" t="s">
+        <v>729</v>
+      </c>
+      <c r="C15" s="162" t="s">
+        <v>726</v>
+      </c>
+      <c r="D15" s="164" t="s">
+        <v>730</v>
+      </c>
+      <c r="E15" s="35">
+        <v>0</v>
+      </c>
+      <c r="F15" s="163" t="s">
+        <v>200</v>
+      </c>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="K15" s="35">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" ht="17" x14ac:dyDescent="0.15">
-      <c r="A10" s="28">
-        <v>2</v>
-      </c>
-      <c r="B10" s="50" t="s">
-        <v>311</v>
-      </c>
-      <c r="C10" s="50" t="s">
-        <v>353</v>
-      </c>
-      <c r="D10" s="47" t="s">
-        <v>313</v>
-      </c>
-      <c r="E10" s="46">
-        <v>1</v>
-      </c>
-      <c r="F10" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="L15" s="35">
+        <f>J15+K15</f>
+        <v>0</v>
+      </c>
+      <c r="M15" s="35">
+        <f>L15-E15</f>
+        <v>0</v>
+      </c>
+      <c r="N15" s="35">
+        <f>(4*E15)-M15</f>
+        <v>0</v>
+      </c>
+      <c r="P15" s="28"/>
+      <c r="Q15" s="28"/>
+      <c r="R15" s="28"/>
+    </row>
+    <row r="16" spans="1:18" s="35" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="35">
+        <v>9</v>
+      </c>
+      <c r="B16" s="162" t="s">
+        <v>228</v>
+      </c>
+      <c r="C16" s="162" t="s">
+        <v>727</v>
+      </c>
+      <c r="D16" s="164" t="s">
+        <v>730</v>
+      </c>
+      <c r="E16" s="35">
+        <v>0</v>
+      </c>
+      <c r="F16" s="163" t="s">
         <v>200</v>
       </c>
-      <c r="G10" s="47" t="s">
-        <v>307</v>
-      </c>
-      <c r="H10" s="47" t="s">
-        <v>337</v>
-      </c>
-      <c r="I10" s="46" t="s">
-        <v>203</v>
-      </c>
-      <c r="J10" s="28">
-        <v>0</v>
-      </c>
-      <c r="K10" s="46">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="L10" s="38">
-        <v>1</v>
-      </c>
-      <c r="M10" s="28">
-        <f>L10-E10</f>
-        <v>0</v>
-      </c>
-      <c r="N10" s="28">
-        <f>(4*E10)-M10</f>
-        <v>4</v>
-      </c>
-      <c r="R10" s="32" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" ht="17" x14ac:dyDescent="0.15">
-      <c r="A11" s="28">
-        <v>9</v>
-      </c>
-      <c r="B11" s="47" t="s">
-        <v>221</v>
-      </c>
-      <c r="C11" s="56" t="s">
-        <v>354</v>
-      </c>
-      <c r="D11" s="46" t="s">
-        <v>319</v>
-      </c>
-      <c r="E11" s="46">
-        <v>1</v>
-      </c>
-      <c r="F11" s="46" t="s">
-        <v>200</v>
-      </c>
-      <c r="G11" s="51" t="s">
-        <v>224</v>
-      </c>
-      <c r="H11" s="46" t="s">
-        <v>332</v>
-      </c>
-      <c r="I11" s="47" t="s">
-        <v>203</v>
-      </c>
-      <c r="J11" s="28">
-        <v>0</v>
-      </c>
-      <c r="K11" s="46">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="L11" s="28">
-        <v>1</v>
-      </c>
-      <c r="M11" s="28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N11" s="28">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="R11" s="32" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" ht="17" x14ac:dyDescent="0.15">
-      <c r="A12" s="28">
-        <v>10</v>
-      </c>
-      <c r="B12" s="47" t="s">
-        <v>269</v>
-      </c>
-      <c r="C12" s="56" t="s">
-        <v>354</v>
-      </c>
-      <c r="D12" s="46" t="s">
-        <v>319</v>
-      </c>
-      <c r="E12" s="46">
-        <v>1</v>
-      </c>
-      <c r="F12" s="46" t="s">
-        <v>200</v>
-      </c>
-      <c r="G12" s="46" t="s">
-        <v>225</v>
-      </c>
-      <c r="H12" s="47" t="s">
-        <v>333</v>
-      </c>
-      <c r="I12" s="47" t="s">
-        <v>203</v>
-      </c>
-      <c r="J12" s="28">
-        <v>0</v>
-      </c>
-      <c r="K12" s="46">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="L12" s="28">
-        <v>1</v>
-      </c>
-      <c r="M12" s="28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N12" s="28">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="R12" s="32" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" ht="17" x14ac:dyDescent="0.15">
-      <c r="A13" s="28">
-        <v>11</v>
-      </c>
-      <c r="B13" s="47" t="s">
-        <v>222</v>
-      </c>
-      <c r="C13" s="56" t="s">
-        <v>354</v>
-      </c>
-      <c r="D13" s="46" t="s">
-        <v>319</v>
-      </c>
-      <c r="E13" s="46">
-        <v>1</v>
-      </c>
-      <c r="F13" s="46" t="s">
-        <v>200</v>
-      </c>
-      <c r="G13" s="46" t="s">
-        <v>226</v>
-      </c>
-      <c r="H13" s="47" t="s">
-        <v>334</v>
-      </c>
-      <c r="I13" s="47" t="s">
-        <v>203</v>
-      </c>
-      <c r="J13" s="28">
-        <v>0</v>
-      </c>
-      <c r="K13" s="46">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="L13" s="28">
-        <v>1</v>
-      </c>
-      <c r="M13" s="28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N13" s="28">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="R13" s="32" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="17" x14ac:dyDescent="0.15">
-      <c r="A14" s="28">
-        <v>12</v>
-      </c>
-      <c r="B14" s="47" t="s">
-        <v>272</v>
-      </c>
-      <c r="C14" s="56" t="s">
-        <v>354</v>
-      </c>
-      <c r="D14" s="46" t="s">
-        <v>319</v>
-      </c>
-      <c r="E14" s="46">
-        <v>1</v>
-      </c>
-      <c r="F14" s="46" t="s">
-        <v>200</v>
-      </c>
-      <c r="G14" s="46" t="s">
-        <v>227</v>
-      </c>
-      <c r="H14" s="47" t="s">
-        <v>335</v>
-      </c>
-      <c r="I14" s="47" t="s">
-        <v>203</v>
-      </c>
-      <c r="J14" s="28">
-        <v>0</v>
-      </c>
-      <c r="K14" s="46">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="L14" s="28">
-        <v>1</v>
-      </c>
-      <c r="M14" s="28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N14" s="28">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="R14" s="32" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="28">
-        <v>13</v>
-      </c>
-      <c r="B15" s="47" t="s">
-        <v>223</v>
-      </c>
-      <c r="C15" s="56" t="s">
-        <v>355</v>
-      </c>
-      <c r="D15" s="51" t="s">
-        <v>340</v>
-      </c>
-      <c r="E15" s="46">
-        <v>1</v>
-      </c>
-      <c r="F15" s="46" t="s">
-        <v>200</v>
-      </c>
-      <c r="G15" s="51" t="s">
-        <v>341</v>
-      </c>
-      <c r="H15" s="47" t="s">
-        <v>336</v>
-      </c>
-      <c r="I15" s="47" t="s">
-        <v>203</v>
-      </c>
-      <c r="J15" s="28">
-        <v>0</v>
-      </c>
-      <c r="K15" s="46">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="L15" s="28">
-        <v>1</v>
-      </c>
-      <c r="M15" s="28">
-        <f>L15-E15</f>
-        <v>0</v>
-      </c>
-      <c r="N15" s="28">
-        <f>(4*E15)-M15</f>
-        <v>4</v>
-      </c>
-      <c r="R15" s="32" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="44" t="s">
-        <v>303</v>
-      </c>
-      <c r="C16" s="44"/>
-      <c r="D16" s="36"/>
-      <c r="F16" s="28"/>
       <c r="G16" s="36"/>
       <c r="H16" s="36"/>
       <c r="K16" s="35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L16" s="35">
@@ -3973,17 +4023,29 @@
       <c r="Q16" s="28"/>
       <c r="R16" s="28"/>
     </row>
-    <row r="17" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="44" t="s">
-        <v>304</v>
-      </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="36"/>
-      <c r="F17" s="28"/>
+    <row r="17" spans="1:18" s="35" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="35">
+        <v>10</v>
+      </c>
+      <c r="B17" s="162" t="s">
+        <v>725</v>
+      </c>
+      <c r="C17" s="162" t="s">
+        <v>728</v>
+      </c>
+      <c r="D17" s="164" t="s">
+        <v>730</v>
+      </c>
+      <c r="E17" s="35">
+        <v>0</v>
+      </c>
+      <c r="F17" s="163" t="s">
+        <v>200</v>
+      </c>
       <c r="G17" s="36"/>
       <c r="H17" s="36"/>
       <c r="K17" s="35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L17" s="35">
@@ -4003,28 +4065,12 @@
       <c r="R17" s="28"/>
     </row>
     <row r="18" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="44" t="s">
-        <v>305</v>
-      </c>
-      <c r="C18" s="44"/>
       <c r="D18" s="36"/>
       <c r="F18" s="28"/>
       <c r="G18" s="36"/>
       <c r="H18" s="36"/>
       <c r="K18" s="35">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L18" s="35">
-        <f>J18+K18</f>
-        <v>0</v>
-      </c>
-      <c r="M18" s="35">
-        <f>L18-E18</f>
-        <v>0</v>
-      </c>
-      <c r="N18" s="35">
-        <f>(4*E18)-M18</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P18" s="28"/>
@@ -4032,9 +4078,7 @@
       <c r="R18" s="28"/>
     </row>
     <row r="19" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="62" t="s">
-        <v>368</v>
-      </c>
+      <c r="B19" s="62"/>
       <c r="C19" s="44"/>
       <c r="D19" s="36"/>
       <c r="F19" s="28"/>
@@ -4044,249 +4088,338 @@
       <c r="Q19" s="28"/>
       <c r="R19" s="28"/>
     </row>
-    <row r="20" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="62" t="s">
-        <v>369</v>
-      </c>
-      <c r="C20" s="44"/>
-      <c r="D20" s="36"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="P20" s="28"/>
-      <c r="Q20" s="28"/>
-      <c r="R20" s="28"/>
-    </row>
-    <row r="21" spans="1:18" s="38" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="57" t="s">
-        <v>371</v>
-      </c>
-      <c r="C21" s="57"/>
-      <c r="D21" s="59"/>
-      <c r="G21" s="59"/>
-      <c r="H21" s="60"/>
-      <c r="I21" s="60"/>
+    <row r="20" spans="1:18" s="38" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="57"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="59"/>
+      <c r="G20" s="59"/>
+      <c r="H20" s="60"/>
+      <c r="I20" s="60"/>
+      <c r="R20" s="39"/>
+    </row>
+    <row r="21" spans="1:18" s="38" customFormat="1" ht="24" x14ac:dyDescent="0.15">
+      <c r="A21" s="104" t="s">
+        <v>432</v>
+      </c>
+      <c r="B21" s="105"/>
+      <c r="C21" s="105"/>
+      <c r="D21" s="105"/>
       <c r="R21" s="39"/>
     </row>
-    <row r="22" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="62"/>
-      <c r="C22" s="44"/>
-      <c r="D22" s="36"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="P22" s="28"/>
-      <c r="Q22" s="28"/>
-      <c r="R22" s="28"/>
-    </row>
-    <row r="23" spans="1:18" s="38" customFormat="1" ht="24" x14ac:dyDescent="0.15">
-      <c r="A23" s="104" t="s">
-        <v>433</v>
-      </c>
-      <c r="B23" s="105"/>
-      <c r="C23" s="105"/>
-      <c r="D23" s="105"/>
-      <c r="R23" s="39"/>
+    <row r="22" spans="1:18" ht="17" x14ac:dyDescent="0.15">
+      <c r="A22" s="28">
+        <v>0</v>
+      </c>
+      <c r="B22" s="46" t="s">
+        <v>142</v>
+      </c>
+      <c r="C22" s="56" t="s">
+        <v>352</v>
+      </c>
+      <c r="D22" s="56" t="s">
+        <v>349</v>
+      </c>
+      <c r="E22" s="46">
+        <v>1</v>
+      </c>
+      <c r="F22" s="46" t="s">
+        <v>200</v>
+      </c>
+      <c r="G22" s="46" t="s">
+        <v>142</v>
+      </c>
+      <c r="H22" s="46" t="s">
+        <v>220</v>
+      </c>
+      <c r="I22" s="46" t="s">
+        <v>203</v>
+      </c>
+      <c r="J22" s="28">
+        <v>0</v>
+      </c>
+      <c r="K22" s="46">
+        <v>10</v>
+      </c>
+      <c r="M22" s="28">
+        <f>L22-E22</f>
+        <v>-1</v>
+      </c>
+      <c r="N22" s="28">
+        <f>(4*E22)-M22</f>
+        <v>5</v>
+      </c>
+      <c r="R22" s="32" t="e">
+        <f t="shared" ref="R22:R29" si="6">Q22/P22</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="17" x14ac:dyDescent="0.15">
+      <c r="A23" s="45">
+        <v>1</v>
+      </c>
+      <c r="B23" s="49" t="s">
+        <v>321</v>
+      </c>
+      <c r="C23" s="49" t="s">
+        <v>353</v>
+      </c>
+      <c r="D23" s="47" t="s">
+        <v>313</v>
+      </c>
+      <c r="E23" s="48">
+        <v>4</v>
+      </c>
+      <c r="F23" s="46" t="s">
+        <v>200</v>
+      </c>
+      <c r="G23" s="46" t="s">
+        <v>201</v>
+      </c>
+      <c r="H23" s="47" t="s">
+        <v>202</v>
+      </c>
+      <c r="I23" s="46" t="s">
+        <v>203</v>
+      </c>
+      <c r="J23" s="28">
+        <v>0</v>
+      </c>
+      <c r="K23" s="46">
+        <f t="shared" ref="K23:K32" si="7">IF(J23&gt;E23,0,E23-J23)</f>
+        <v>4</v>
+      </c>
+      <c r="L23" s="38">
+        <v>10</v>
+      </c>
+      <c r="M23" s="28">
+        <f t="shared" ref="M23:M28" si="8">L23-E23</f>
+        <v>6</v>
+      </c>
+      <c r="N23" s="28">
+        <f t="shared" ref="N23:N28" si="9">(4*E23)-M23</f>
+        <v>10</v>
+      </c>
+      <c r="R23" s="32" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="24" spans="1:18" ht="17" x14ac:dyDescent="0.15">
-      <c r="A24" s="45" t="s">
-        <v>322</v>
-      </c>
-      <c r="B24" s="56" t="s">
-        <v>351</v>
-      </c>
-      <c r="C24" s="56" t="s">
-        <v>360</v>
+      <c r="A24" s="28">
+        <v>2</v>
+      </c>
+      <c r="B24" s="50" t="s">
+        <v>311</v>
+      </c>
+      <c r="C24" s="50" t="s">
+        <v>353</v>
       </c>
       <c r="D24" s="47" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="E24" s="46">
-        <v>0</v>
-      </c>
-      <c r="F24" s="47" t="s">
-        <v>325</v>
+        <v>1</v>
+      </c>
+      <c r="F24" s="46" t="s">
+        <v>200</v>
       </c>
       <c r="G24" s="47" t="s">
-        <v>326</v>
+        <v>307</v>
       </c>
       <c r="H24" s="47" t="s">
-        <v>324</v>
-      </c>
-      <c r="I24" s="47" t="s">
-        <v>324</v>
-      </c>
-      <c r="J24" s="52" t="s">
-        <v>325</v>
-      </c>
-      <c r="K24" s="54" t="s">
-        <v>325</v>
-      </c>
-      <c r="L24" s="52"/>
-      <c r="M24" s="52" t="s">
-        <v>325</v>
-      </c>
-      <c r="N24" s="52" t="s">
-        <v>325</v>
-      </c>
-      <c r="R24" s="32"/>
-    </row>
-    <row r="25" spans="1:18" ht="68" x14ac:dyDescent="0.15">
-      <c r="A25" s="45" t="s">
-        <v>314</v>
-      </c>
-      <c r="B25" s="46" t="s">
-        <v>217</v>
-      </c>
-      <c r="C25" s="150" t="s">
-        <v>356</v>
-      </c>
-      <c r="D25" s="51" t="s">
-        <v>348</v>
+        <v>337</v>
+      </c>
+      <c r="I24" s="46" t="s">
+        <v>203</v>
+      </c>
+      <c r="J24" s="28">
+        <v>0</v>
+      </c>
+      <c r="K24" s="46">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="L24" s="38">
+        <v>1</v>
+      </c>
+      <c r="M24" s="28">
+        <f>L24-E24</f>
+        <v>0</v>
+      </c>
+      <c r="N24" s="28">
+        <f>(4*E24)-M24</f>
+        <v>4</v>
+      </c>
+      <c r="R24" s="32" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="17" x14ac:dyDescent="0.15">
+      <c r="A25" s="28">
+        <v>9</v>
+      </c>
+      <c r="B25" s="47" t="s">
+        <v>221</v>
+      </c>
+      <c r="C25" s="56" t="s">
+        <v>354</v>
+      </c>
+      <c r="D25" s="46" t="s">
+        <v>319</v>
       </c>
       <c r="E25" s="46">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" s="46" t="s">
         <v>200</v>
       </c>
-      <c r="G25" s="47" t="s">
-        <v>218</v>
-      </c>
-      <c r="H25" s="47" t="s">
-        <v>329</v>
-      </c>
-      <c r="I25" s="46" t="s">
+      <c r="G25" s="51" t="s">
+        <v>224</v>
+      </c>
+      <c r="H25" s="46" t="s">
+        <v>332</v>
+      </c>
+      <c r="I25" s="47" t="s">
         <v>203</v>
       </c>
       <c r="J25" s="28">
         <v>0</v>
       </c>
-      <c r="K25" s="53">
-        <f t="shared" ref="K25:K30" si="4">IF(J25&gt;E25,0,E25-J25)</f>
-        <v>2</v>
+      <c r="K25" s="46">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="L25" s="28">
+        <v>1</v>
       </c>
       <c r="M25" s="28">
-        <f>L25-E25</f>
-        <v>-2</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="N25" s="28">
-        <f>(4*E25)-M25</f>
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="R25" s="32" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="17" x14ac:dyDescent="0.15">
+      <c r="A26" s="28">
         <v>10</v>
       </c>
-      <c r="R25" s="32" t="e">
-        <f>Q25/P25</f>
+      <c r="B26" s="47" t="s">
+        <v>269</v>
+      </c>
+      <c r="C26" s="56" t="s">
+        <v>354</v>
+      </c>
+      <c r="D26" s="46" t="s">
+        <v>319</v>
+      </c>
+      <c r="E26" s="46">
+        <v>1</v>
+      </c>
+      <c r="F26" s="46" t="s">
+        <v>200</v>
+      </c>
+      <c r="G26" s="46" t="s">
+        <v>225</v>
+      </c>
+      <c r="H26" s="47" t="s">
+        <v>333</v>
+      </c>
+      <c r="I26" s="47" t="s">
+        <v>203</v>
+      </c>
+      <c r="J26" s="28">
+        <v>0</v>
+      </c>
+      <c r="K26" s="46">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="L26" s="28">
+        <v>1</v>
+      </c>
+      <c r="M26" s="28">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="N26" s="28">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="R26" s="32" t="e">
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="26" spans="1:18" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
-      <c r="A26" s="87" t="s">
-        <v>315</v>
-      </c>
-      <c r="B26" s="30" t="s">
-        <v>217</v>
-      </c>
-      <c r="C26" s="149" t="s">
-        <v>357</v>
-      </c>
-      <c r="D26" s="87" t="s">
-        <v>316</v>
-      </c>
-      <c r="E26" s="30">
-        <v>4</v>
-      </c>
-      <c r="F26" s="30" t="s">
-        <v>200</v>
-      </c>
-      <c r="G26" s="88" t="s">
-        <v>331</v>
-      </c>
-      <c r="H26" s="87" t="s">
-        <v>330</v>
-      </c>
-      <c r="I26" s="88" t="s">
-        <v>203</v>
-      </c>
-      <c r="J26" s="30">
-        <v>0</v>
-      </c>
-      <c r="K26" s="30">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="L26" s="30">
-        <v>4</v>
-      </c>
-      <c r="M26" s="30">
-        <f>L26-E26</f>
-        <v>0</v>
-      </c>
-      <c r="N26" s="30">
-        <f>(4*E26)-M26</f>
-        <v>16</v>
-      </c>
-      <c r="R26" s="89"/>
-    </row>
-    <row r="27" spans="1:18" s="46" customFormat="1" ht="34" x14ac:dyDescent="0.15">
-      <c r="A27" s="51" t="s">
-        <v>344</v>
-      </c>
-      <c r="B27" s="46" t="s">
-        <v>217</v>
+    <row r="27" spans="1:18" ht="17" x14ac:dyDescent="0.15">
+      <c r="A27" s="28">
+        <v>11</v>
+      </c>
+      <c r="B27" s="47" t="s">
+        <v>222</v>
       </c>
       <c r="C27" s="56" t="s">
-        <v>357</v>
-      </c>
-      <c r="D27" s="51" t="s">
-        <v>342</v>
+        <v>354</v>
+      </c>
+      <c r="D27" s="46" t="s">
+        <v>319</v>
       </c>
       <c r="E27" s="46">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F27" s="46" t="s">
         <v>200</v>
       </c>
-      <c r="G27" s="47" t="s">
-        <v>338</v>
+      <c r="G27" s="46" t="s">
+        <v>226</v>
       </c>
       <c r="H27" s="47" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="I27" s="47" t="s">
-        <v>219</v>
-      </c>
-      <c r="J27" s="46">
+        <v>203</v>
+      </c>
+      <c r="J27" s="28">
         <v>0</v>
       </c>
       <c r="K27" s="46">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="L27" s="28">
+        <v>1</v>
+      </c>
+      <c r="M27" s="28">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="N27" s="28">
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
-      <c r="L27" s="46">
-        <v>4</v>
-      </c>
-      <c r="M27" s="46">
-        <f t="shared" ref="M27:M32" si="5">L27-E27</f>
-        <v>0</v>
-      </c>
-      <c r="N27" s="46">
-        <f t="shared" ref="N27:N32" si="6">(4*E27)-M27</f>
-        <v>16</v>
-      </c>
-      <c r="R27" s="90"/>
+      <c r="R27" s="32" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="28" spans="1:18" ht="17" x14ac:dyDescent="0.15">
       <c r="A28" s="28">
-        <v>15</v>
-      </c>
-      <c r="B28" s="46" t="s">
-        <v>228</v>
+        <v>12</v>
+      </c>
+      <c r="B28" s="47" t="s">
+        <v>272</v>
       </c>
       <c r="C28" s="56" t="s">
-        <v>358</v>
-      </c>
-      <c r="D28" s="51" t="s">
-        <v>346</v>
+        <v>354</v>
+      </c>
+      <c r="D28" s="46" t="s">
+        <v>319</v>
       </c>
       <c r="E28" s="46">
         <v>1</v>
@@ -4294,571 +4427,1004 @@
       <c r="F28" s="46" t="s">
         <v>200</v>
       </c>
-      <c r="G28" s="47" t="s">
-        <v>229</v>
+      <c r="G28" s="46" t="s">
+        <v>227</v>
       </c>
       <c r="H28" s="47" t="s">
-        <v>328</v>
-      </c>
-      <c r="I28" s="51" t="s">
+        <v>335</v>
+      </c>
+      <c r="I28" s="47" t="s">
         <v>203</v>
       </c>
       <c r="J28" s="28">
-        <v>1</v>
-      </c>
-      <c r="K28" s="53">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K28" s="46">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="L28" s="28">
+        <v>1</v>
       </c>
       <c r="M28" s="28">
-        <f t="shared" si="5"/>
-        <v>-1</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="N28" s="28">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="R28" s="32" t="e">
         <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="R28" s="32" t="e">
-        <f>Q28/P28</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="85" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:18" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="28">
-        <v>101</v>
-      </c>
-      <c r="B29" s="46" t="s">
-        <v>204</v>
-      </c>
-      <c r="C29" s="46" t="s">
-        <v>140</v>
-      </c>
-      <c r="D29" s="46" t="s">
-        <v>140</v>
+        <v>13</v>
+      </c>
+      <c r="B29" s="47" t="s">
+        <v>223</v>
+      </c>
+      <c r="C29" s="56" t="s">
+        <v>355</v>
+      </c>
+      <c r="D29" s="51" t="s">
+        <v>340</v>
       </c>
       <c r="E29" s="46">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="F29" s="46" t="s">
         <v>200</v>
       </c>
-      <c r="G29" s="46" t="s">
+      <c r="G29" s="51" t="s">
+        <v>341</v>
+      </c>
+      <c r="H29" s="47" t="s">
+        <v>336</v>
+      </c>
+      <c r="I29" s="47" t="s">
+        <v>203</v>
+      </c>
+      <c r="J29" s="28">
+        <v>0</v>
+      </c>
+      <c r="K29" s="46">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="L29" s="28">
+        <v>1</v>
+      </c>
+      <c r="M29" s="28">
+        <f>L29-E29</f>
+        <v>0</v>
+      </c>
+      <c r="N29" s="28">
+        <f>(4*E29)-M29</f>
+        <v>4</v>
+      </c>
+      <c r="R29" s="32" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="44" t="s">
+        <v>303</v>
+      </c>
+      <c r="C30" s="44"/>
+      <c r="D30" s="36"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="36"/>
+      <c r="K30" s="35">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L30" s="35">
+        <f>J30+K30</f>
+        <v>0</v>
+      </c>
+      <c r="M30" s="35">
+        <f>L30-E30</f>
+        <v>0</v>
+      </c>
+      <c r="N30" s="35">
+        <f>(4*E30)-M30</f>
+        <v>0</v>
+      </c>
+      <c r="P30" s="28"/>
+      <c r="Q30" s="28"/>
+      <c r="R30" s="28"/>
+    </row>
+    <row r="31" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="44" t="s">
+        <v>304</v>
+      </c>
+      <c r="C31" s="44"/>
+      <c r="D31" s="36"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="36"/>
+      <c r="H31" s="36"/>
+      <c r="K31" s="35">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L31" s="35">
+        <f>J31+K31</f>
+        <v>0</v>
+      </c>
+      <c r="M31" s="35">
+        <f>L31-E31</f>
+        <v>0</v>
+      </c>
+      <c r="N31" s="35">
+        <f>(4*E31)-M31</f>
+        <v>0</v>
+      </c>
+      <c r="P31" s="28"/>
+      <c r="Q31" s="28"/>
+      <c r="R31" s="28"/>
+    </row>
+    <row r="32" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="44" t="s">
+        <v>305</v>
+      </c>
+      <c r="C32" s="44"/>
+      <c r="D32" s="36"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="36"/>
+      <c r="H32" s="36"/>
+      <c r="K32" s="35">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L32" s="35">
+        <f>J32+K32</f>
+        <v>0</v>
+      </c>
+      <c r="M32" s="35">
+        <f>L32-E32</f>
+        <v>0</v>
+      </c>
+      <c r="N32" s="35">
+        <f>(4*E32)-M32</f>
+        <v>0</v>
+      </c>
+      <c r="P32" s="28"/>
+      <c r="Q32" s="28"/>
+      <c r="R32" s="28"/>
+    </row>
+    <row r="33" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="62" t="s">
+        <v>368</v>
+      </c>
+      <c r="C33" s="44"/>
+      <c r="D33" s="36"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="36"/>
+      <c r="H33" s="36"/>
+      <c r="P33" s="28"/>
+      <c r="Q33" s="28"/>
+      <c r="R33" s="28"/>
+    </row>
+    <row r="34" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="62" t="s">
+        <v>369</v>
+      </c>
+      <c r="C34" s="44"/>
+      <c r="D34" s="36"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="36"/>
+      <c r="H34" s="36"/>
+      <c r="P34" s="28"/>
+      <c r="Q34" s="28"/>
+      <c r="R34" s="28"/>
+    </row>
+    <row r="35" spans="1:18" s="38" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B35" s="57" t="s">
+        <v>371</v>
+      </c>
+      <c r="C35" s="57"/>
+      <c r="D35" s="59"/>
+      <c r="G35" s="59"/>
+      <c r="H35" s="60"/>
+      <c r="I35" s="60"/>
+      <c r="R35" s="39"/>
+    </row>
+    <row r="36" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="62"/>
+      <c r="C36" s="44"/>
+      <c r="D36" s="36"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="36"/>
+      <c r="H36" s="36"/>
+      <c r="P36" s="28"/>
+      <c r="Q36" s="28"/>
+      <c r="R36" s="28"/>
+    </row>
+    <row r="37" spans="1:18" s="38" customFormat="1" ht="24" x14ac:dyDescent="0.15">
+      <c r="A37" s="104" t="s">
+        <v>433</v>
+      </c>
+      <c r="B37" s="105"/>
+      <c r="C37" s="105"/>
+      <c r="D37" s="105"/>
+      <c r="R37" s="39"/>
+    </row>
+    <row r="38" spans="1:18" ht="17" x14ac:dyDescent="0.15">
+      <c r="A38" s="45" t="s">
+        <v>322</v>
+      </c>
+      <c r="B38" s="56" t="s">
+        <v>351</v>
+      </c>
+      <c r="C38" s="56" t="s">
+        <v>360</v>
+      </c>
+      <c r="D38" s="47" t="s">
+        <v>323</v>
+      </c>
+      <c r="E38" s="46">
+        <v>0</v>
+      </c>
+      <c r="F38" s="47" t="s">
+        <v>325</v>
+      </c>
+      <c r="G38" s="47" t="s">
+        <v>326</v>
+      </c>
+      <c r="H38" s="47" t="s">
+        <v>324</v>
+      </c>
+      <c r="I38" s="47" t="s">
+        <v>324</v>
+      </c>
+      <c r="J38" s="52" t="s">
+        <v>325</v>
+      </c>
+      <c r="K38" s="54" t="s">
+        <v>325</v>
+      </c>
+      <c r="L38" s="52"/>
+      <c r="M38" s="52" t="s">
+        <v>325</v>
+      </c>
+      <c r="N38" s="52" t="s">
+        <v>325</v>
+      </c>
+      <c r="R38" s="32"/>
+    </row>
+    <row r="39" spans="1:18" ht="68" x14ac:dyDescent="0.15">
+      <c r="A39" s="45" t="s">
+        <v>314</v>
+      </c>
+      <c r="B39" s="46" t="s">
+        <v>217</v>
+      </c>
+      <c r="C39" s="150" t="s">
+        <v>356</v>
+      </c>
+      <c r="D39" s="51" t="s">
+        <v>348</v>
+      </c>
+      <c r="E39" s="46">
+        <v>2</v>
+      </c>
+      <c r="F39" s="46" t="s">
+        <v>200</v>
+      </c>
+      <c r="G39" s="47" t="s">
+        <v>218</v>
+      </c>
+      <c r="H39" s="47" t="s">
+        <v>329</v>
+      </c>
+      <c r="I39" s="46" t="s">
+        <v>203</v>
+      </c>
+      <c r="J39" s="28">
+        <v>0</v>
+      </c>
+      <c r="K39" s="53">
+        <f t="shared" ref="K39:K44" si="10">IF(J39&gt;E39,0,E39-J39)</f>
+        <v>2</v>
+      </c>
+      <c r="M39" s="28">
+        <f>L39-E39</f>
+        <v>-2</v>
+      </c>
+      <c r="N39" s="28">
+        <f>(4*E39)-M39</f>
+        <v>10</v>
+      </c>
+      <c r="R39" s="32" t="e">
+        <f>Q39/P39</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" s="30" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+      <c r="A40" s="87" t="s">
+        <v>315</v>
+      </c>
+      <c r="B40" s="30" t="s">
+        <v>217</v>
+      </c>
+      <c r="C40" s="149" t="s">
+        <v>357</v>
+      </c>
+      <c r="D40" s="87" t="s">
+        <v>316</v>
+      </c>
+      <c r="E40" s="30">
+        <v>4</v>
+      </c>
+      <c r="F40" s="30" t="s">
+        <v>200</v>
+      </c>
+      <c r="G40" s="88" t="s">
+        <v>331</v>
+      </c>
+      <c r="H40" s="87" t="s">
+        <v>330</v>
+      </c>
+      <c r="I40" s="88" t="s">
+        <v>203</v>
+      </c>
+      <c r="J40" s="30">
+        <v>0</v>
+      </c>
+      <c r="K40" s="30">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="L40" s="30">
+        <v>4</v>
+      </c>
+      <c r="M40" s="30">
+        <f>L40-E40</f>
+        <v>0</v>
+      </c>
+      <c r="N40" s="30">
+        <f>(4*E40)-M40</f>
+        <v>16</v>
+      </c>
+      <c r="R40" s="89"/>
+    </row>
+    <row r="41" spans="1:18" s="46" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+      <c r="A41" s="51" t="s">
+        <v>344</v>
+      </c>
+      <c r="B41" s="46" t="s">
+        <v>217</v>
+      </c>
+      <c r="C41" s="56" t="s">
+        <v>357</v>
+      </c>
+      <c r="D41" s="51" t="s">
+        <v>342</v>
+      </c>
+      <c r="E41" s="46">
+        <v>4</v>
+      </c>
+      <c r="F41" s="46" t="s">
+        <v>200</v>
+      </c>
+      <c r="G41" s="47" t="s">
+        <v>338</v>
+      </c>
+      <c r="H41" s="47" t="s">
+        <v>339</v>
+      </c>
+      <c r="I41" s="47" t="s">
+        <v>219</v>
+      </c>
+      <c r="J41" s="46">
+        <v>0</v>
+      </c>
+      <c r="K41" s="46">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="L41" s="46">
+        <v>4</v>
+      </c>
+      <c r="M41" s="46">
+        <f t="shared" ref="M41:M46" si="11">L41-E41</f>
+        <v>0</v>
+      </c>
+      <c r="N41" s="46">
+        <f t="shared" ref="N41:N46" si="12">(4*E41)-M41</f>
+        <v>16</v>
+      </c>
+      <c r="R41" s="90"/>
+    </row>
+    <row r="42" spans="1:18" ht="17" x14ac:dyDescent="0.15">
+      <c r="A42" s="28">
+        <v>15</v>
+      </c>
+      <c r="B42" s="46" t="s">
+        <v>228</v>
+      </c>
+      <c r="C42" s="56" t="s">
+        <v>358</v>
+      </c>
+      <c r="D42" s="51" t="s">
+        <v>346</v>
+      </c>
+      <c r="E42" s="46">
+        <v>1</v>
+      </c>
+      <c r="F42" s="46" t="s">
+        <v>200</v>
+      </c>
+      <c r="G42" s="47" t="s">
+        <v>229</v>
+      </c>
+      <c r="H42" s="47" t="s">
+        <v>328</v>
+      </c>
+      <c r="I42" s="51" t="s">
+        <v>203</v>
+      </c>
+      <c r="J42" s="28">
+        <v>1</v>
+      </c>
+      <c r="K42" s="53">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="M42" s="28">
+        <f t="shared" si="11"/>
+        <v>-1</v>
+      </c>
+      <c r="N42" s="28">
+        <f t="shared" si="12"/>
+        <v>5</v>
+      </c>
+      <c r="R42" s="32" t="e">
+        <f>Q42/P42</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" ht="85" x14ac:dyDescent="0.15">
+      <c r="A43" s="28">
+        <v>101</v>
+      </c>
+      <c r="B43" s="46" t="s">
+        <v>204</v>
+      </c>
+      <c r="C43" s="46" t="s">
+        <v>140</v>
+      </c>
+      <c r="D43" s="46" t="s">
+        <v>140</v>
+      </c>
+      <c r="E43" s="46">
+        <v>70</v>
+      </c>
+      <c r="F43" s="46" t="s">
+        <v>200</v>
+      </c>
+      <c r="G43" s="46" t="s">
         <v>205</v>
       </c>
-      <c r="H29" s="46" t="s">
+      <c r="H43" s="46" t="s">
         <v>206</v>
       </c>
-      <c r="I29" s="46" t="s">
+      <c r="I43" s="46" t="s">
         <v>203</v>
       </c>
-      <c r="J29" s="28">
+      <c r="J43" s="28">
         <v>860</v>
       </c>
-      <c r="K29" s="53">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L29" s="28">
-        <f>J29+K29</f>
+      <c r="K43" s="53">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="L43" s="28">
+        <f>J43+K43</f>
         <v>860</v>
       </c>
-      <c r="M29" s="28">
-        <f t="shared" si="5"/>
+      <c r="M43" s="28">
+        <f t="shared" si="11"/>
         <v>790</v>
       </c>
-      <c r="N29" s="28">
-        <f t="shared" si="6"/>
+      <c r="N43" s="28">
+        <f t="shared" si="12"/>
         <v>-510</v>
       </c>
-      <c r="R29" s="32" t="e">
-        <f>Q29/P29</f>
+      <c r="R43" s="32" t="e">
+        <f>Q43/P43</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="102" x14ac:dyDescent="0.15">
-      <c r="A30" s="28">
+    <row r="44" spans="1:18" ht="102" x14ac:dyDescent="0.15">
+      <c r="A44" s="28">
         <v>102</v>
       </c>
-      <c r="B30" s="46" t="s">
+      <c r="B44" s="46" t="s">
         <v>207</v>
       </c>
-      <c r="C30" s="46" t="s">
+      <c r="C44" s="46" t="s">
         <v>208</v>
       </c>
-      <c r="D30" s="46" t="s">
+      <c r="D44" s="46" t="s">
         <v>208</v>
       </c>
-      <c r="E30" s="46">
+      <c r="E44" s="46">
         <v>0.8</v>
       </c>
-      <c r="F30" s="46" t="s">
+      <c r="F44" s="46" t="s">
         <v>209</v>
       </c>
-      <c r="G30" s="46" t="s">
+      <c r="G44" s="46" t="s">
         <v>210</v>
       </c>
-      <c r="H30" s="46" t="s">
+      <c r="H44" s="46" t="s">
         <v>211</v>
       </c>
-      <c r="I30" s="46" t="s">
+      <c r="I44" s="46" t="s">
         <v>203</v>
       </c>
-      <c r="J30" s="28">
+      <c r="J44" s="28">
         <v>426.2</v>
       </c>
-      <c r="K30" s="53">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L30" s="28">
-        <f>J30+K30</f>
+      <c r="K44" s="53">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="L44" s="28">
+        <f>J44+K44</f>
         <v>426.2</v>
       </c>
-      <c r="M30" s="28">
-        <f t="shared" si="5"/>
+      <c r="M44" s="28">
+        <f t="shared" si="11"/>
         <v>425.4</v>
       </c>
-      <c r="N30" s="28">
-        <f t="shared" si="6"/>
+      <c r="N44" s="28">
+        <f t="shared" si="12"/>
         <v>-422.2</v>
       </c>
-      <c r="P30" s="28">
+      <c r="P44" s="28">
         <v>430</v>
       </c>
-      <c r="R30" s="32">
-        <f>Q30/P30</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" ht="85" x14ac:dyDescent="0.15">
-      <c r="A31" s="28">
+      <c r="R44" s="32">
+        <f>Q44/P44</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" ht="85" x14ac:dyDescent="0.15">
+      <c r="A45" s="28">
         <v>103</v>
       </c>
-      <c r="B31" s="46" t="s">
+      <c r="B45" s="46" t="s">
         <v>207</v>
       </c>
-      <c r="C31" s="46" t="s">
+      <c r="C45" s="46" t="s">
         <v>208</v>
       </c>
-      <c r="D31" s="46" t="s">
+      <c r="D45" s="46" t="s">
         <v>208</v>
       </c>
-      <c r="E31" s="46">
+      <c r="E45" s="46">
         <v>0.8</v>
       </c>
-      <c r="F31" s="46" t="s">
+      <c r="F45" s="46" t="s">
         <v>209</v>
       </c>
-      <c r="G31" s="46" t="s">
+      <c r="G45" s="46" t="s">
         <v>212</v>
       </c>
-      <c r="H31" s="46" t="s">
+      <c r="H45" s="46" t="s">
         <v>213</v>
       </c>
-      <c r="I31" s="46" t="s">
+      <c r="I45" s="46" t="s">
         <v>203</v>
       </c>
-      <c r="J31" s="33">
+      <c r="J45" s="33">
         <v>100</v>
       </c>
-      <c r="K31" s="55">
-        <v>0</v>
-      </c>
-      <c r="L31" s="28">
-        <f>J31+K31</f>
+      <c r="K45" s="55">
+        <v>0</v>
+      </c>
+      <c r="L45" s="28">
+        <f>J45+K45</f>
         <v>100</v>
       </c>
-      <c r="M31" s="28">
-        <f t="shared" si="5"/>
+      <c r="M45" s="28">
+        <f t="shared" si="11"/>
         <v>99.2</v>
       </c>
-      <c r="N31" s="28">
-        <f t="shared" si="6"/>
+      <c r="N45" s="28">
+        <f t="shared" si="12"/>
         <v>-96</v>
       </c>
-      <c r="P31" s="28">
+      <c r="P45" s="28">
         <v>100</v>
       </c>
-      <c r="Q31" s="34">
+      <c r="Q45" s="34">
         <v>6.49</v>
       </c>
-      <c r="R31" s="32">
-        <f>Q31/P31</f>
+      <c r="R45" s="32">
+        <f>Q45/P45</f>
         <v>6.4899999999999999E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="68" x14ac:dyDescent="0.15">
-      <c r="A32" s="28">
+    <row r="46" spans="1:18" ht="68" x14ac:dyDescent="0.15">
+      <c r="A46" s="28">
         <v>104</v>
       </c>
-      <c r="B32" s="46" t="s">
+      <c r="B46" s="46" t="s">
         <v>207</v>
       </c>
-      <c r="C32" s="46" t="s">
+      <c r="C46" s="46" t="s">
         <v>214</v>
       </c>
-      <c r="D32" s="46" t="s">
+      <c r="D46" s="46" t="s">
         <v>214</v>
       </c>
-      <c r="E32" s="46">
+      <c r="E46" s="46">
         <v>0.75</v>
       </c>
-      <c r="F32" s="46" t="s">
+      <c r="F46" s="46" t="s">
         <v>209</v>
       </c>
-      <c r="G32" s="46" t="s">
+      <c r="G46" s="46" t="s">
         <v>215</v>
       </c>
-      <c r="H32" s="46" t="s">
+      <c r="H46" s="46" t="s">
         <v>216</v>
       </c>
-      <c r="I32" s="46" t="s">
+      <c r="I46" s="46" t="s">
         <v>203</v>
       </c>
-      <c r="J32" s="33">
+      <c r="J46" s="33">
         <v>747</v>
       </c>
-      <c r="K32" s="55">
-        <v>0</v>
-      </c>
-      <c r="L32" s="33">
-        <f>J32+K32</f>
+      <c r="K46" s="55">
+        <v>0</v>
+      </c>
+      <c r="L46" s="33">
+        <f>J46+K46</f>
         <v>747</v>
       </c>
-      <c r="M32" s="33">
-        <f t="shared" si="5"/>
+      <c r="M46" s="33">
+        <f t="shared" si="11"/>
         <v>746.25</v>
       </c>
-      <c r="N32" s="33">
-        <f t="shared" si="6"/>
+      <c r="N46" s="33">
+        <f t="shared" si="12"/>
         <v>-743.25</v>
       </c>
-      <c r="P32" s="28">
+      <c r="P46" s="28">
         <v>747</v>
       </c>
-      <c r="Q32" s="34">
+      <c r="Q46" s="34">
         <f>12.65+3.95+1.18</f>
         <v>17.78</v>
       </c>
-      <c r="R32" s="32">
-        <f>Q32/P32</f>
+      <c r="R46" s="32">
+        <f>Q46/P46</f>
         <v>2.3801874163319948E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:18" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="91" t="s">
+    <row r="47" spans="1:18" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="91" t="s">
         <v>597</v>
       </c>
-      <c r="B33" s="115"/>
-      <c r="E33" s="110"/>
-      <c r="F33" s="28"/>
-      <c r="H33" s="118"/>
-    </row>
-    <row r="34" spans="1:18" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="27"/>
-      <c r="B34" s="151" t="s">
+      <c r="B47" s="115"/>
+      <c r="E47" s="110"/>
+      <c r="F47" s="28"/>
+      <c r="H47" s="118"/>
+    </row>
+    <row r="48" spans="1:18" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="27"/>
+      <c r="B48" s="151" t="s">
         <v>217</v>
       </c>
-      <c r="C34" s="23" t="s">
+      <c r="C48" s="23" t="s">
         <v>356</v>
       </c>
-      <c r="D34" s="50" t="s">
+      <c r="D48" s="50" t="s">
         <v>682</v>
       </c>
-      <c r="E34" s="152">
+      <c r="E48" s="152">
         <v>2</v>
       </c>
-      <c r="F34" s="46"/>
-      <c r="G34" s="50"/>
-      <c r="H34" s="153" t="s">
+      <c r="F48" s="46"/>
+      <c r="G48" s="50"/>
+      <c r="H48" s="153" t="s">
         <v>687</v>
       </c>
     </row>
-    <row r="35" spans="1:18" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="27"/>
-      <c r="B35" s="116" t="s">
+    <row r="49" spans="1:18" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="27"/>
+      <c r="B49" s="116" t="s">
         <v>217</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C49" t="s">
         <v>356</v>
       </c>
-      <c r="D35" s="26" t="s">
+      <c r="D49" s="26" t="s">
         <v>683</v>
       </c>
-      <c r="E35" s="110">
+      <c r="E49" s="110">
         <v>4</v>
       </c>
-      <c r="F35" s="28"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="119"/>
-    </row>
-    <row r="36" spans="1:18" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="148" t="s">
+      <c r="F49" s="28"/>
+      <c r="G49" s="26"/>
+      <c r="H49" s="119"/>
+    </row>
+    <row r="50" spans="1:18" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="148" t="s">
         <v>680</v>
       </c>
-      <c r="B36" s="116"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="110"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="26"/>
-      <c r="H36" s="119"/>
-    </row>
-    <row r="37" spans="1:18" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="C37" s="97" t="s">
+      <c r="B50" s="116"/>
+      <c r="D50" s="26"/>
+      <c r="E50" s="110"/>
+      <c r="F50" s="28"/>
+      <c r="G50" s="26"/>
+      <c r="H50" s="119"/>
+    </row>
+    <row r="51" spans="1:18" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="C51" s="97" t="s">
         <v>438</v>
       </c>
-      <c r="J37" s="40"/>
-      <c r="K37" s="40"/>
-      <c r="L37" s="40"/>
-      <c r="M37" s="40"/>
-      <c r="N37" s="40"/>
-      <c r="Q37" s="41"/>
-      <c r="R37" s="39"/>
-    </row>
-    <row r="38" spans="1:18" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="C38" s="97" t="s">
+      <c r="J51" s="40"/>
+      <c r="K51" s="40"/>
+      <c r="L51" s="40"/>
+      <c r="M51" s="40"/>
+      <c r="N51" s="40"/>
+      <c r="Q51" s="41"/>
+      <c r="R51" s="39"/>
+    </row>
+    <row r="52" spans="1:18" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="C52" s="97" t="s">
         <v>435</v>
       </c>
-      <c r="J38" s="40"/>
-      <c r="K38" s="40"/>
-      <c r="L38" s="40"/>
-      <c r="M38" s="40"/>
-      <c r="N38" s="40"/>
-      <c r="Q38" s="41"/>
-      <c r="R38" s="39"/>
-    </row>
-    <row r="39" spans="1:18" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="C39" s="97" t="s">
+      <c r="J52" s="40"/>
+      <c r="K52" s="40"/>
+      <c r="L52" s="40"/>
+      <c r="M52" s="40"/>
+      <c r="N52" s="40"/>
+      <c r="Q52" s="41"/>
+      <c r="R52" s="39"/>
+    </row>
+    <row r="53" spans="1:18" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="C53" s="97" t="s">
         <v>436</v>
       </c>
-      <c r="J39" s="40"/>
-      <c r="K39" s="40"/>
-      <c r="L39" s="40"/>
-      <c r="M39" s="40"/>
-      <c r="N39" s="40"/>
-      <c r="Q39" s="41"/>
-      <c r="R39" s="39"/>
-    </row>
-    <row r="40" spans="1:18" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="C40" s="97" t="s">
+      <c r="J53" s="40"/>
+      <c r="K53" s="40"/>
+      <c r="L53" s="40"/>
+      <c r="M53" s="40"/>
+      <c r="N53" s="40"/>
+      <c r="Q53" s="41"/>
+      <c r="R53" s="39"/>
+    </row>
+    <row r="54" spans="1:18" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="C54" s="97" t="s">
         <v>437</v>
       </c>
-      <c r="J40" s="40"/>
-      <c r="K40" s="40"/>
-      <c r="L40" s="40"/>
-      <c r="M40" s="40"/>
-      <c r="N40" s="40"/>
-      <c r="Q40" s="41"/>
-      <c r="R40" s="39"/>
-    </row>
-    <row r="41" spans="1:18" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="C41" s="57" t="s">
+      <c r="J54" s="40"/>
+      <c r="K54" s="40"/>
+      <c r="L54" s="40"/>
+      <c r="M54" s="40"/>
+      <c r="N54" s="40"/>
+      <c r="Q54" s="41"/>
+      <c r="R54" s="39"/>
+    </row>
+    <row r="55" spans="1:18" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="C55" s="57" t="s">
         <v>372</v>
       </c>
-      <c r="J41" s="40"/>
-      <c r="K41" s="40"/>
-      <c r="L41" s="40"/>
-      <c r="M41" s="40"/>
-      <c r="N41" s="40"/>
-      <c r="Q41" s="41"/>
-      <c r="R41" s="39"/>
-    </row>
-    <row r="42" spans="1:18" s="38" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B42" s="57"/>
-      <c r="C42" s="94" t="s">
+      <c r="J55" s="40"/>
+      <c r="K55" s="40"/>
+      <c r="L55" s="40"/>
+      <c r="M55" s="40"/>
+      <c r="N55" s="40"/>
+      <c r="Q55" s="41"/>
+      <c r="R55" s="39"/>
+    </row>
+    <row r="56" spans="1:18" s="38" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B56" s="57"/>
+      <c r="C56" s="94" t="s">
         <v>587</v>
       </c>
-      <c r="J42" s="40"/>
-      <c r="K42" s="40"/>
-      <c r="L42" s="40"/>
-      <c r="M42" s="40"/>
-      <c r="N42" s="40"/>
-      <c r="Q42" s="41"/>
-      <c r="R42" s="39"/>
-    </row>
-    <row r="43" spans="1:18" s="38" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B43" s="57"/>
-      <c r="J43" s="40"/>
-      <c r="K43" s="40"/>
-      <c r="L43" s="40"/>
-      <c r="M43" s="40"/>
-      <c r="N43" s="40"/>
-      <c r="Q43" s="41"/>
-      <c r="R43" s="39"/>
-    </row>
-    <row r="44" spans="1:18" s="38" customFormat="1" ht="24" x14ac:dyDescent="0.15">
-      <c r="A44" s="104" t="s">
+      <c r="J56" s="40"/>
+      <c r="K56" s="40"/>
+      <c r="L56" s="40"/>
+      <c r="M56" s="40"/>
+      <c r="N56" s="40"/>
+      <c r="Q56" s="41"/>
+      <c r="R56" s="39"/>
+    </row>
+    <row r="57" spans="1:18" s="38" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B57" s="57"/>
+      <c r="J57" s="40"/>
+      <c r="K57" s="40"/>
+      <c r="L57" s="40"/>
+      <c r="M57" s="40"/>
+      <c r="N57" s="40"/>
+      <c r="Q57" s="41"/>
+      <c r="R57" s="39"/>
+    </row>
+    <row r="58" spans="1:18" s="38" customFormat="1" ht="24" x14ac:dyDescent="0.15">
+      <c r="A58" s="104" t="s">
         <v>434</v>
       </c>
-      <c r="B44" s="105"/>
-      <c r="C44" s="105"/>
-      <c r="D44" s="106"/>
-      <c r="G44" s="60"/>
-      <c r="H44" s="60"/>
-      <c r="I44" s="59"/>
-      <c r="R44" s="39"/>
-    </row>
-    <row r="45" spans="1:18" ht="17" x14ac:dyDescent="0.15">
-      <c r="B45" s="92" t="s">
+      <c r="B58" s="105"/>
+      <c r="C58" s="105"/>
+      <c r="D58" s="106"/>
+      <c r="G58" s="60"/>
+      <c r="H58" s="60"/>
+      <c r="I58" s="59"/>
+      <c r="R58" s="39"/>
+    </row>
+    <row r="59" spans="1:18" ht="17" x14ac:dyDescent="0.15">
+      <c r="B59" s="92" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="48" spans="1:18" ht="24" x14ac:dyDescent="0.15">
-      <c r="A48" s="104" t="s">
+    <row r="62" spans="1:18" ht="24" x14ac:dyDescent="0.15">
+      <c r="A62" s="104" t="s">
         <v>572</v>
       </c>
-      <c r="B48" s="105"/>
-      <c r="C48" s="105"/>
-      <c r="D48" s="106"/>
-    </row>
-    <row r="49" spans="1:18" ht="17" x14ac:dyDescent="0.15">
-      <c r="D49" s="145" t="s">
+      <c r="B62" s="105"/>
+      <c r="C62" s="105"/>
+      <c r="D62" s="106"/>
+    </row>
+    <row r="63" spans="1:18" ht="17" x14ac:dyDescent="0.15">
+      <c r="D63" s="145" t="s">
         <v>690</v>
       </c>
-      <c r="E49" s="28">
+      <c r="E63" s="28">
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:18" ht="34" x14ac:dyDescent="0.15">
-      <c r="A50" s="28">
+    <row r="64" spans="1:18" ht="34" x14ac:dyDescent="0.15">
+      <c r="A64" s="28">
         <v>14</v>
       </c>
-      <c r="B50" s="47" t="s">
+      <c r="B64" s="47" t="s">
         <v>317</v>
       </c>
-      <c r="C50" s="56" t="s">
+      <c r="C64" s="56" t="s">
         <v>359</v>
       </c>
-      <c r="D50" s="51" t="s">
+      <c r="D64" s="51" t="s">
         <v>345</v>
       </c>
-      <c r="E50" s="46">
+      <c r="E64" s="46">
         <v>14</v>
       </c>
-      <c r="F50" s="46" t="s">
+      <c r="F64" s="46" t="s">
         <v>200</v>
       </c>
-      <c r="G50" s="47" t="s">
+      <c r="G64" s="47" t="s">
         <v>318</v>
       </c>
-      <c r="H50" s="47" t="s">
+      <c r="H64" s="47" t="s">
         <v>327</v>
       </c>
-      <c r="I50" s="47" t="s">
+      <c r="I64" s="47" t="s">
         <v>219</v>
       </c>
-      <c r="J50" s="28">
-        <v>0</v>
-      </c>
-      <c r="K50" s="46">
-        <f>IF(J50&gt;E50,0,E50-J50)</f>
+      <c r="J64" s="28">
+        <v>0</v>
+      </c>
+      <c r="K64" s="46">
+        <f>IF(J64&gt;E64,0,E64-J64)</f>
         <v>14</v>
       </c>
-      <c r="L50" s="28">
+      <c r="L64" s="28">
         <v>4</v>
       </c>
-      <c r="M50" s="28">
-        <f>L50-E50</f>
+      <c r="M64" s="28">
+        <f>L64-E64</f>
         <v>-10</v>
       </c>
-      <c r="N50" s="28">
-        <f>(4*E50)-M50</f>
+      <c r="N64" s="28">
+        <f>(4*E64)-M64</f>
         <v>66</v>
       </c>
-      <c r="R50" s="32" t="e">
-        <f>Q50/P50</f>
+      <c r="R64" s="32" t="e">
+        <f>Q64/P64</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="51" spans="1:18" ht="34" x14ac:dyDescent="0.15">
-      <c r="A51" s="45">
+    <row r="65" spans="1:18" ht="34" x14ac:dyDescent="0.15">
+      <c r="A65" s="45">
         <v>16</v>
       </c>
-      <c r="B51" s="49" t="s">
+      <c r="B65" s="49" t="s">
         <v>320</v>
       </c>
-      <c r="C51" s="56" t="s">
+      <c r="C65" s="56" t="s">
         <v>359</v>
       </c>
-      <c r="D51" s="51" t="s">
+      <c r="D65" s="51" t="s">
         <v>343</v>
       </c>
-      <c r="E51" s="48">
+      <c r="E65" s="48">
         <v>14</v>
       </c>
-      <c r="F51" s="46" t="s">
+      <c r="F65" s="46" t="s">
         <v>200</v>
       </c>
-      <c r="G51" s="46" t="s">
+      <c r="G65" s="46" t="s">
         <v>201</v>
       </c>
-      <c r="H51" s="47" t="s">
+      <c r="H65" s="47" t="s">
         <v>202</v>
       </c>
-      <c r="I51" s="47" t="s">
+      <c r="I65" s="47" t="s">
         <v>219</v>
       </c>
-      <c r="J51" s="28">
-        <v>0</v>
-      </c>
-      <c r="K51" s="46">
-        <f>IF(J51&gt;E51,0,E51-J51)</f>
+      <c r="J65" s="28">
+        <v>0</v>
+      </c>
+      <c r="K65" s="46">
+        <f>IF(J65&gt;E65,0,E65-J65)</f>
         <v>14</v>
       </c>
-      <c r="L51" s="38">
-        <v>0</v>
-      </c>
-      <c r="M51" s="28">
-        <f>L51-E51</f>
+      <c r="L65" s="38">
+        <v>0</v>
+      </c>
+      <c r="M65" s="28">
+        <f>L65-E65</f>
         <v>-14</v>
       </c>
-      <c r="N51" s="28">
-        <f>(4*E51)-M51</f>
+      <c r="N65" s="28">
+        <f>(4*E65)-M65</f>
         <v>70</v>
       </c>
-      <c r="R51" s="32" t="e">
-        <f>Q51/P51</f>
+      <c r="R65" s="32" t="e">
+        <f>Q65/P65</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A52" s="45"/>
-      <c r="B52" s="49"/>
-      <c r="C52" s="56"/>
-      <c r="D52" s="51"/>
-      <c r="E52" s="48"/>
-      <c r="F52" s="46"/>
-      <c r="G52" s="46"/>
-      <c r="H52" s="47"/>
-      <c r="I52" s="47"/>
-      <c r="K52" s="46"/>
-      <c r="L52" s="38"/>
-      <c r="R52" s="32"/>
-    </row>
-    <row r="53" spans="1:18" ht="68" x14ac:dyDescent="0.15">
-      <c r="D53" s="93" t="s">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A66" s="45"/>
+      <c r="B66" s="49"/>
+      <c r="C66" s="56"/>
+      <c r="D66" s="51"/>
+      <c r="E66" s="48"/>
+      <c r="F66" s="46"/>
+      <c r="G66" s="46"/>
+      <c r="H66" s="47"/>
+      <c r="I66" s="47"/>
+      <c r="K66" s="46"/>
+      <c r="L66" s="38"/>
+      <c r="R66" s="32"/>
+    </row>
+    <row r="67" spans="1:18" ht="68" x14ac:dyDescent="0.15">
+      <c r="D67" s="93" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="54" spans="1:18" ht="17" x14ac:dyDescent="0.15">
-      <c r="D54" s="145" t="s">
+    <row r="68" spans="1:18" ht="17" x14ac:dyDescent="0.15">
+      <c r="D68" s="145" t="s">
         <v>691</v>
       </c>
-      <c r="E54" s="28">
+      <c r="E68" s="28">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A6:N59" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:N59">
-      <sortCondition ref="B6:B59"/>
+  <autoFilter ref="A6:N73" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:N73">
+      <sortCondition ref="B6:B73"/>
     </sortState>
   </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="P3:R3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H34" r:id="rId1" xr:uid="{CC20020E-09E9-1145-A0B9-91ED22861541}"/>
+    <hyperlink ref="H48" r:id="rId1" xr:uid="{CC20020E-09E9-1145-A0B9-91ED22861541}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -4868,7 +5434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1052A41E-3EA7-B148-953B-E2218E71D84C}">
   <dimension ref="A1:AE118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" ySplit="10" topLeftCell="B72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
@@ -4941,11 +5507,11 @@
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.15">
-      <c r="P7" s="154" t="s">
+      <c r="P7" s="161" t="s">
         <v>173</v>
       </c>
-      <c r="Q7" s="154"/>
-      <c r="R7" s="154"/>
+      <c r="Q7" s="161"/>
+      <c r="R7" s="161"/>
     </row>
     <row r="8" spans="1:31" s="83" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A8" s="83" t="s">
@@ -6705,17 +7271,17 @@
     <row r="80" spans="1:18" s="83" customFormat="1" ht="21" x14ac:dyDescent="0.15">
       <c r="B80" s="113"/>
       <c r="C80" s="68"/>
-      <c r="D80" s="160" t="s">
+      <c r="D80" s="159" t="s">
         <v>723</v>
       </c>
       <c r="E80" s="85">
         <v>1</v>
       </c>
-      <c r="F80" s="159" t="s">
+      <c r="F80" s="158" t="s">
         <v>200</v>
       </c>
       <c r="G80" s="84"/>
-      <c r="H80" s="161" t="s">
+      <c r="H80" s="160" t="s">
         <v>722</v>
       </c>
       <c r="K80" s="38"/>
@@ -6729,7 +7295,7 @@
     <row r="81" spans="1:20" ht="17" x14ac:dyDescent="0.15">
       <c r="B81" s="69"/>
       <c r="C81" s="68"/>
-      <c r="D81" s="156" t="s">
+      <c r="D81" s="155" t="s">
         <v>721</v>
       </c>
       <c r="E81" s="64">
@@ -7439,7 +8005,7 @@
   <mergeCells count="1">
     <mergeCell ref="P7:R7"/>
   </mergeCells>
-  <phoneticPr fontId="18" type="noConversion"/>
+  <phoneticPr fontId="19" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="H22" r:id="rId1" xr:uid="{B3564F39-BDFC-024B-80FC-3B84D3B19B84}"/>
     <hyperlink ref="H19" r:id="rId2" xr:uid="{441A81FD-7638-214B-A580-55099579328C}"/>
@@ -7528,11 +8094,11 @@
       <c r="A3" s="29"/>
       <c r="B3" s="27"/>
       <c r="C3" s="27"/>
-      <c r="P3" s="154" t="s">
+      <c r="P3" s="161" t="s">
         <v>173</v>
       </c>
-      <c r="Q3" s="154"/>
-      <c r="R3" s="154"/>
+      <c r="Q3" s="161"/>
+      <c r="R3" s="161"/>
     </row>
     <row r="4" spans="1:18" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" s="29"/>
@@ -7672,7 +8238,7 @@
       <c r="G9" s="81" t="s">
         <v>393</v>
       </c>
-      <c r="H9" s="155" t="s">
+      <c r="H9" s="154" t="s">
         <v>362</v>
       </c>
       <c r="I9" s="79" t="s">
@@ -7813,7 +8379,7 @@
       <c r="G16" s="56" t="s">
         <v>376</v>
       </c>
-      <c r="H16" s="158" t="s">
+      <c r="H16" s="157" t="s">
         <v>375</v>
       </c>
       <c r="J16" s="71">
@@ -7845,7 +8411,7 @@
     </row>
     <row r="18" spans="1:18" s="27" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="B18" s="73"/>
-      <c r="C18" s="157" t="s">
+      <c r="C18" s="156" t="s">
         <v>697</v>
       </c>
       <c r="D18" s="28"/>
@@ -7858,10 +8424,10 @@
       <c r="G18" s="27" t="s">
         <v>699</v>
       </c>
-      <c r="H18" s="157" t="s">
+      <c r="H18" s="156" t="s">
         <v>698</v>
       </c>
-      <c r="I18" s="157" t="s">
+      <c r="I18" s="156" t="s">
         <v>397</v>
       </c>
       <c r="J18" s="27">
@@ -7903,7 +8469,7 @@
         <v>579</v>
       </c>
       <c r="H19" s="28"/>
-      <c r="I19" s="157" t="s">
+      <c r="I19" s="156" t="s">
         <v>397</v>
       </c>
       <c r="J19" s="27">
@@ -7930,7 +8496,7 @@
       <c r="H20" s="117" t="s">
         <v>702</v>
       </c>
-      <c r="I20" s="157" t="s">
+      <c r="I20" s="156" t="s">
         <v>397</v>
       </c>
       <c r="J20" s="27">
@@ -7941,7 +8507,7 @@
       <c r="R20" s="28"/>
     </row>
     <row r="21" spans="1:18" s="27" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="C21" s="157" t="s">
+      <c r="C21" s="156" t="s">
         <v>700</v>
       </c>
       <c r="D21" s="28"/>
@@ -7957,7 +8523,7 @@
       <c r="H21" s="117" t="s">
         <v>701</v>
       </c>
-      <c r="I21" s="157" t="s">
+      <c r="I21" s="156" t="s">
         <v>397</v>
       </c>
       <c r="J21" s="27">
@@ -7968,7 +8534,7 @@
       <c r="R21" s="28"/>
     </row>
     <row r="22" spans="1:18" s="27" customFormat="1" ht="17" x14ac:dyDescent="0.15">
-      <c r="C22" s="157" t="s">
+      <c r="C22" s="156" t="s">
         <v>695</v>
       </c>
       <c r="D22" s="28"/>
@@ -7984,7 +8550,7 @@
       <c r="H22" s="117" t="s">
         <v>694</v>
       </c>
-      <c r="I22" s="157" t="s">
+      <c r="I22" s="156" t="s">
         <v>397</v>
       </c>
       <c r="J22" s="27">
@@ -8011,7 +8577,7 @@
       <c r="H23" s="117" t="s">
         <v>703</v>
       </c>
-      <c r="I23" s="157" t="s">
+      <c r="I23" s="156" t="s">
         <v>397</v>
       </c>
       <c r="P23" s="28"/>
@@ -8026,7 +8592,7 @@
       <c r="F24" s="28"/>
       <c r="G24" s="28"/>
       <c r="H24" s="28"/>
-      <c r="I24" s="157" t="s">
+      <c r="I24" s="156" t="s">
         <v>397</v>
       </c>
       <c r="P24" s="28"/>
@@ -8041,7 +8607,7 @@
       <c r="F25" s="28"/>
       <c r="G25" s="28"/>
       <c r="H25" s="28"/>
-      <c r="I25" s="157" t="s">
+      <c r="I25" s="156" t="s">
         <v>397</v>
       </c>
       <c r="P25" s="28"/>
@@ -8058,7 +8624,7 @@
         <v>582</v>
       </c>
       <c r="H26" s="28"/>
-      <c r="I26" s="157" t="s">
+      <c r="I26" s="156" t="s">
         <v>397</v>
       </c>
       <c r="P26" s="28"/>
@@ -8075,7 +8641,7 @@
         <v>423</v>
       </c>
       <c r="H27" s="28"/>
-      <c r="I27" s="157" t="s">
+      <c r="I27" s="156" t="s">
         <v>397</v>
       </c>
       <c r="P27" s="28"/>
@@ -8177,7 +8743,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" ht="17" x14ac:dyDescent="0.15">
-      <c r="C40" s="156" t="s">
+      <c r="C40" s="155" t="s">
         <v>706</v>
       </c>
       <c r="E40" s="28">
@@ -8188,7 +8754,7 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="17" x14ac:dyDescent="0.15">
-      <c r="C41" s="156" t="s">
+      <c r="C41" s="155" t="s">
         <v>711</v>
       </c>
       <c r="E41" s="28">
@@ -8197,7 +8763,7 @@
       <c r="H41" s="117"/>
     </row>
     <row r="42" spans="1:9" ht="17" x14ac:dyDescent="0.15">
-      <c r="C42" s="156" t="s">
+      <c r="C42" s="155" t="s">
         <v>712</v>
       </c>
       <c r="E42" s="28">

</xml_diff>

<commit_message>
Update BOM as assembled LB V0.4
</commit_message>
<xml_diff>
--- a/Manufacturing/BOM Core 64 v0.4.0 CB Yellow LB Blue.xlsx
+++ b/Manufacturing/BOM Core 64 v0.4.0 CB Yellow LB Blue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Manufacturing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24DA3A7-BBD2-7E4E-91A6-A1DFC18B1488}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4725F46F-5F46-4446-AD51-20437620F0F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="34660" windowHeight="22680" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1277" uniqueCount="750">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1291" uniqueCount="750">
   <si>
     <t>Digi-Key Part Number</t>
   </si>
@@ -2315,10 +2315,17 @@
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -2473,7 +2480,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2514,6 +2521,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -2590,37 +2603,37 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="179">
+  <cellXfs count="181">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="44" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="19" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="18" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="17" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2630,196 +2643,341 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="15" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="16" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="17" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="17" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="4" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" xfId="4" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="4" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2827,244 +2985,105 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="4" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="16" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="4" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" xfId="4" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="4" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="4" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3563,11 +3582,11 @@
         <v>172</v>
       </c>
       <c r="C3" s="27"/>
-      <c r="P3" s="165" t="s">
+      <c r="P3" s="178" t="s">
         <v>173</v>
       </c>
-      <c r="Q3" s="165"/>
-      <c r="R3" s="165"/>
+      <c r="Q3" s="178"/>
+      <c r="R3" s="178"/>
     </row>
     <row r="4" spans="1:18" ht="51" x14ac:dyDescent="0.15">
       <c r="A4" s="29"/>
@@ -5532,10 +5551,10 @@
   <dimension ref="A1:AF121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="10" topLeftCell="C72" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="10" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="H83" sqref="H83"/>
+      <selection pane="bottomRight" activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
@@ -5611,11 +5630,11 @@
       <c r="B6" s="92"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="Q7" s="165" t="s">
+      <c r="Q7" s="178" t="s">
         <v>173</v>
       </c>
-      <c r="R7" s="165"/>
-      <c r="S7" s="165"/>
+      <c r="R7" s="178"/>
+      <c r="S7" s="178"/>
     </row>
     <row r="8" spans="1:32" s="83" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A8" s="83" t="s">
@@ -5678,7 +5697,7 @@
       <c r="A10" s="83" t="s">
         <v>286</v>
       </c>
-      <c r="B10" s="168" t="s">
+      <c r="B10" s="167" t="s">
         <v>724</v>
       </c>
       <c r="C10" s="38" t="s">
@@ -5774,7 +5793,7 @@
       <c r="A11" s="104" t="s">
         <v>428</v>
       </c>
-      <c r="B11" s="169"/>
+      <c r="B11" s="168"/>
       <c r="C11" s="105"/>
       <c r="D11" s="105"/>
       <c r="F11" s="86"/>
@@ -5783,7 +5802,7 @@
     </row>
     <row r="12" spans="1:32" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A12" s="27"/>
-      <c r="B12" s="173" t="s">
+      <c r="B12" s="172" t="s">
         <v>726</v>
       </c>
       <c r="C12" s="115" t="s">
@@ -5808,7 +5827,7 @@
     </row>
     <row r="13" spans="1:32" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A13" s="27"/>
-      <c r="B13" s="173" t="s">
+      <c r="B13" s="172" t="s">
         <v>726</v>
       </c>
       <c r="C13" s="116" t="s">
@@ -5833,7 +5852,7 @@
     </row>
     <row r="14" spans="1:32" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A14" s="27"/>
-      <c r="B14" s="173" t="s">
+      <c r="B14" s="172" t="s">
         <v>726</v>
       </c>
       <c r="C14" s="116" t="s">
@@ -5856,9 +5875,11 @@
         <v>602</v>
       </c>
     </row>
-    <row r="15" spans="1:32" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:32" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A15" s="27"/>
-      <c r="B15" s="46"/>
+      <c r="B15" s="179" t="s">
+        <v>726</v>
+      </c>
       <c r="C15" s="115" t="s">
         <v>448</v>
       </c>
@@ -5881,7 +5902,7 @@
     </row>
     <row r="16" spans="1:32" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A16" s="27"/>
-      <c r="B16" s="173" t="s">
+      <c r="B16" s="172" t="s">
         <v>732</v>
       </c>
       <c r="C16" s="115" t="s">
@@ -5904,9 +5925,11 @@
         <v>598</v>
       </c>
     </row>
-    <row r="17" spans="1:9" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A17" s="27"/>
-      <c r="B17" s="46"/>
+      <c r="B17" s="179" t="s">
+        <v>726</v>
+      </c>
       <c r="C17" s="116" t="s">
         <v>452</v>
       </c>
@@ -5927,9 +5950,11 @@
         <v>606</v>
       </c>
     </row>
-    <row r="18" spans="1:9" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A18" s="27"/>
-      <c r="B18" s="46"/>
+      <c r="B18" s="179" t="s">
+        <v>726</v>
+      </c>
       <c r="C18" s="116" t="s">
         <v>454</v>
       </c>
@@ -5952,7 +5977,7 @@
     </row>
     <row r="19" spans="1:9" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A19" s="27"/>
-      <c r="B19" s="173" t="s">
+      <c r="B19" s="172" t="s">
         <v>726</v>
       </c>
       <c r="C19" s="115" t="s">
@@ -5977,7 +6002,7 @@
     </row>
     <row r="20" spans="1:9" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A20" s="27"/>
-      <c r="B20" s="173" t="s">
+      <c r="B20" s="172" t="s">
         <v>726</v>
       </c>
       <c r="C20" s="115" t="s">
@@ -6002,7 +6027,7 @@
     </row>
     <row r="21" spans="1:9" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A21" s="27"/>
-      <c r="B21" s="173" t="s">
+      <c r="B21" s="172" t="s">
         <v>725</v>
       </c>
       <c r="C21" s="115" t="s">
@@ -6025,9 +6050,11 @@
         <v>594</v>
       </c>
     </row>
-    <row r="22" spans="1:9" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A22" s="27"/>
-      <c r="B22" s="46"/>
+      <c r="B22" s="172" t="s">
+        <v>726</v>
+      </c>
       <c r="C22" s="116" t="s">
         <v>521</v>
       </c>
@@ -6048,9 +6075,11 @@
         <v>631</v>
       </c>
     </row>
-    <row r="23" spans="1:9" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A23" s="27"/>
-      <c r="B23" s="46"/>
+      <c r="B23" s="172" t="s">
+        <v>726</v>
+      </c>
       <c r="C23" s="116" t="s">
         <v>522</v>
       </c>
@@ -6071,9 +6100,11 @@
         <v>632</v>
       </c>
     </row>
-    <row r="24" spans="1:9" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A24" s="27"/>
-      <c r="B24" s="46"/>
+      <c r="B24" s="172" t="s">
+        <v>726</v>
+      </c>
       <c r="C24" s="115" t="s">
         <v>523</v>
       </c>
@@ -6096,7 +6127,7 @@
     </row>
     <row r="25" spans="1:9" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A25" s="27"/>
-      <c r="B25" s="173" t="s">
+      <c r="B25" s="172" t="s">
         <v>731</v>
       </c>
       <c r="C25" s="115" t="s">
@@ -6121,7 +6152,7 @@
     </row>
     <row r="26" spans="1:9" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A26" s="27"/>
-      <c r="B26" s="173" t="s">
+      <c r="B26" s="172" t="s">
         <v>726</v>
       </c>
       <c r="C26" s="116" t="s">
@@ -6144,7 +6175,7 @@
     </row>
     <row r="27" spans="1:9" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A27" s="27"/>
-      <c r="B27" s="173" t="s">
+      <c r="B27" s="172" t="s">
         <v>726</v>
       </c>
       <c r="C27" s="115" t="s">
@@ -6165,9 +6196,11 @@
         <v>635</v>
       </c>
     </row>
-    <row r="28" spans="1:9" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:9" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A28" s="27"/>
-      <c r="B28" s="46"/>
+      <c r="B28" s="172" t="s">
+        <v>726</v>
+      </c>
       <c r="C28" s="116" t="s">
         <v>531</v>
       </c>
@@ -6186,9 +6219,11 @@
         <v>648</v>
       </c>
     </row>
-    <row r="29" spans="1:9" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:9" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A29" s="27"/>
-      <c r="B29" s="46"/>
+      <c r="B29" s="180" t="s">
+        <v>726</v>
+      </c>
       <c r="C29" s="116" t="s">
         <v>532</v>
       </c>
@@ -6207,9 +6242,11 @@
         <v>646</v>
       </c>
     </row>
-    <row r="30" spans="1:9" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:9" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A30" s="27"/>
-      <c r="B30" s="46"/>
+      <c r="B30" s="179" t="s">
+        <v>726</v>
+      </c>
       <c r="C30" s="115" t="s">
         <v>533</v>
       </c>
@@ -6228,9 +6265,11 @@
         <v>641</v>
       </c>
     </row>
-    <row r="31" spans="1:9" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:9" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A31" s="27"/>
-      <c r="B31" s="46"/>
+      <c r="B31" s="179" t="s">
+        <v>726</v>
+      </c>
       <c r="C31" s="116" t="s">
         <v>534</v>
       </c>
@@ -6251,7 +6290,7 @@
     </row>
     <row r="32" spans="1:9" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A32" s="27"/>
-      <c r="B32" s="173" t="s">
+      <c r="B32" s="172" t="s">
         <v>726</v>
       </c>
       <c r="C32" s="115" t="s">
@@ -6272,9 +6311,11 @@
         <v>636</v>
       </c>
     </row>
-    <row r="33" spans="1:19" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:19" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A33" s="27"/>
-      <c r="B33" s="46"/>
+      <c r="B33" s="179" t="s">
+        <v>726</v>
+      </c>
       <c r="C33" s="115" t="s">
         <v>537</v>
       </c>
@@ -6293,9 +6334,11 @@
         <v>638</v>
       </c>
     </row>
-    <row r="34" spans="1:19" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:19" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A34" s="27"/>
-      <c r="B34" s="46"/>
+      <c r="B34" s="179" t="s">
+        <v>726</v>
+      </c>
       <c r="C34" s="115" t="s">
         <v>539</v>
       </c>
@@ -6314,9 +6357,9 @@
         <v>639</v>
       </c>
     </row>
-    <row r="35" spans="1:19" customFormat="1" ht="34" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:19" customFormat="1" ht="51" x14ac:dyDescent="0.15">
       <c r="A35" s="27"/>
-      <c r="B35" s="173" t="s">
+      <c r="B35" s="172" t="s">
         <v>729</v>
       </c>
       <c r="C35" s="115" t="s">
@@ -6341,7 +6384,7 @@
     </row>
     <row r="36" spans="1:19" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A36" s="27"/>
-      <c r="B36" s="173" t="s">
+      <c r="B36" s="172" t="s">
         <v>726</v>
       </c>
       <c r="C36" s="115" t="s">
@@ -6366,7 +6409,7 @@
     </row>
     <row r="37" spans="1:19" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A37" s="27"/>
-      <c r="B37" s="173" t="s">
+      <c r="B37" s="172" t="s">
         <v>726</v>
       </c>
       <c r="C37" s="115" t="s">
@@ -6389,9 +6432,11 @@
         <v>651</v>
       </c>
     </row>
-    <row r="38" spans="1:19" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:19" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A38" s="27"/>
-      <c r="B38" s="46"/>
+      <c r="B38" s="179" t="s">
+        <v>726</v>
+      </c>
       <c r="C38" s="115" t="s">
         <v>548</v>
       </c>
@@ -6412,9 +6457,11 @@
         <v>652</v>
       </c>
     </row>
-    <row r="39" spans="1:19" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:19" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A39" s="27"/>
-      <c r="B39" s="46"/>
+      <c r="B39" s="179" t="s">
+        <v>726</v>
+      </c>
       <c r="C39" s="115" t="s">
         <v>553</v>
       </c>
@@ -6457,7 +6504,7 @@
     </row>
     <row r="41" spans="1:19" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A41" s="27"/>
-      <c r="B41" s="173" t="s">
+      <c r="B41" s="172" t="s">
         <v>726</v>
       </c>
       <c r="C41" s="115" t="s">
@@ -7223,7 +7270,7 @@
     </row>
     <row r="69" spans="1:19" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A69" s="27"/>
-      <c r="B69" s="173" t="s">
+      <c r="B69" s="172" t="s">
         <v>726</v>
       </c>
       <c r="C69" s="115" t="s">
@@ -7257,7 +7304,7 @@
     </row>
     <row r="70" spans="1:19" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A70" s="27"/>
-      <c r="B70" s="173" t="s">
+      <c r="B70" s="172" t="s">
         <v>737</v>
       </c>
       <c r="C70" s="115" t="s">
@@ -7280,7 +7327,7 @@
     </row>
     <row r="71" spans="1:19" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A71" s="27"/>
-      <c r="B71" s="173" t="s">
+      <c r="B71" s="172" t="s">
         <v>737</v>
       </c>
       <c r="C71" s="115" t="s">
@@ -7302,7 +7349,7 @@
     </row>
     <row r="72" spans="1:19" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A72" s="27"/>
-      <c r="B72" s="173" t="s">
+      <c r="B72" s="172" t="s">
         <v>737</v>
       </c>
       <c r="C72" s="115" t="s">
@@ -7452,7 +7499,7 @@
         <v>481</v>
       </c>
       <c r="D77"/>
-      <c r="E77" s="170" t="s">
+      <c r="E77" s="169" t="s">
         <v>742</v>
       </c>
       <c r="F77" s="85">
@@ -7491,7 +7538,7 @@
       <c r="A79" s="104" t="s">
         <v>429</v>
       </c>
-      <c r="B79" s="169"/>
+      <c r="B79" s="168"/>
       <c r="C79" s="105"/>
       <c r="D79" s="105"/>
       <c r="F79" s="86"/>
@@ -7500,7 +7547,7 @@
     </row>
     <row r="80" spans="1:19" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A80" s="27"/>
-      <c r="B80" s="173" t="s">
+      <c r="B80" s="172" t="s">
         <v>726</v>
       </c>
       <c r="C80" s="116" t="s">
@@ -7525,7 +7572,7 @@
     </row>
     <row r="81" spans="1:21" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A81" s="27"/>
-      <c r="B81" s="173" t="s">
+      <c r="B81" s="172" t="s">
         <v>726</v>
       </c>
       <c r="C81" s="115" t="s">
@@ -7549,7 +7596,7 @@
       </c>
     </row>
     <row r="82" spans="1:21" s="83" customFormat="1" ht="22" x14ac:dyDescent="0.15">
-      <c r="B82" s="173" t="s">
+      <c r="B82" s="172" t="s">
         <v>726</v>
       </c>
       <c r="C82" s="113" t="s">
@@ -7570,12 +7617,12 @@
       <c r="S82" s="38"/>
     </row>
     <row r="83" spans="1:21" s="83" customFormat="1" ht="21" x14ac:dyDescent="0.15">
-      <c r="B83" s="173" t="s">
+      <c r="B83" s="172" t="s">
         <v>730</v>
       </c>
       <c r="C83" s="113"/>
       <c r="D83" s="68"/>
-      <c r="E83" s="166" t="s">
+      <c r="E83" s="165" t="s">
         <v>728</v>
       </c>
       <c r="F83" s="85">
@@ -7597,7 +7644,7 @@
       <c r="S83" s="38"/>
     </row>
     <row r="84" spans="1:21" ht="17" x14ac:dyDescent="0.15">
-      <c r="B84" s="173" t="s">
+      <c r="B84" s="172" t="s">
         <v>726</v>
       </c>
       <c r="C84" s="69"/>
@@ -7614,7 +7661,7 @@
     </row>
     <row r="85" spans="1:21" s="123" customFormat="1" ht="24" x14ac:dyDescent="0.15">
       <c r="A85" s="121"/>
-      <c r="B85" s="171"/>
+      <c r="B85" s="170"/>
       <c r="C85" s="122" t="s">
         <v>615</v>
       </c>
@@ -7629,7 +7676,7 @@
       <c r="A86" s="133" t="s">
         <v>268</v>
       </c>
-      <c r="B86" s="178" t="s">
+      <c r="B86" s="177" t="s">
         <v>726</v>
       </c>
       <c r="C86" s="123"/>
@@ -7684,7 +7731,7 @@
       <c r="A87" s="133" t="s">
         <v>619</v>
       </c>
-      <c r="B87" s="178" t="s">
+      <c r="B87" s="177" t="s">
         <v>726</v>
       </c>
       <c r="C87" s="122"/>
@@ -7719,7 +7766,7 @@
       <c r="A88" s="133" t="s">
         <v>620</v>
       </c>
-      <c r="B88" s="178" t="s">
+      <c r="B88" s="177" t="s">
         <v>726</v>
       </c>
       <c r="C88" s="123"/>
@@ -8123,7 +8170,7 @@
       <c r="A104" s="98">
         <v>307</v>
       </c>
-      <c r="B104" s="172"/>
+      <c r="B104" s="171"/>
       <c r="C104" s="92" t="s">
         <v>283</v>
       </c>
@@ -8334,7 +8381,7 @@
   <mergeCells count="1">
     <mergeCell ref="Q7:S7"/>
   </mergeCells>
-  <phoneticPr fontId="20" type="noConversion"/>
+  <phoneticPr fontId="21" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="I21" r:id="rId1" xr:uid="{B3564F39-BDFC-024B-80FC-3B84D3B19B84}"/>
     <hyperlink ref="I19" r:id="rId2" xr:uid="{441A81FD-7638-214B-A580-55099579328C}"/>
@@ -8427,11 +8474,11 @@
       <c r="B3" s="29"/>
       <c r="C3" s="27"/>
       <c r="D3" s="27"/>
-      <c r="Q3" s="165" t="s">
+      <c r="Q3" s="178" t="s">
         <v>173</v>
       </c>
-      <c r="R3" s="165"/>
-      <c r="S3" s="165"/>
+      <c r="R3" s="178"/>
+      <c r="S3" s="178"/>
     </row>
     <row r="4" spans="1:19" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" s="29"/>
@@ -8478,7 +8525,7 @@
       <c r="A6" s="28" t="s">
         <v>186</v>
       </c>
-      <c r="B6" s="170" t="s">
+      <c r="B6" s="169" t="s">
         <v>724</v>
       </c>
       <c r="C6" s="28" t="s">
@@ -8534,7 +8581,7 @@
       <c r="A7" s="58" t="s">
         <v>349</v>
       </c>
-      <c r="B7" s="175"/>
+      <c r="B7" s="174"/>
       <c r="E7" s="59"/>
       <c r="H7" s="60"/>
       <c r="I7" s="60"/>
@@ -8543,7 +8590,7 @@
     </row>
     <row r="8" spans="1:19" s="38" customFormat="1" ht="24" x14ac:dyDescent="0.15">
       <c r="A8" s="58"/>
-      <c r="B8" s="174"/>
+      <c r="B8" s="173"/>
       <c r="C8" s="82" t="s">
         <v>688</v>
       </c>
@@ -8698,13 +8745,13 @@
       <c r="S15" s="28"/>
     </row>
     <row r="16" spans="1:19" s="65" customFormat="1" ht="34" x14ac:dyDescent="0.15">
-      <c r="B16" s="177" t="s">
+      <c r="B16" s="176" t="s">
         <v>726</v>
       </c>
-      <c r="D16" s="176" t="s">
+      <c r="D16" s="175" t="s">
         <v>372</v>
       </c>
-      <c r="E16" s="177" t="s">
+      <c r="E16" s="176" t="s">
         <v>749</v>
       </c>
       <c r="F16" s="66">
@@ -8905,10 +8952,10 @@
     </row>
     <row r="23" spans="1:19" s="27" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="B23" s="46"/>
-      <c r="C23" s="167" t="s">
+      <c r="C23" s="166" t="s">
         <v>740</v>
       </c>
-      <c r="D23" s="167" t="s">
+      <c r="D23" s="166" t="s">
         <v>746</v>
       </c>
       <c r="E23" s="28"/>
@@ -8933,19 +8980,19 @@
     </row>
     <row r="24" spans="1:19" s="27" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="B24" s="46"/>
-      <c r="C24" s="167" t="s">
+      <c r="C24" s="166" t="s">
         <v>739</v>
       </c>
-      <c r="D24" s="167" t="s">
+      <c r="D24" s="166" t="s">
         <v>738</v>
       </c>
-      <c r="E24" s="170" t="s">
+      <c r="E24" s="169" t="s">
         <v>745</v>
       </c>
       <c r="F24" s="27">
         <v>2</v>
       </c>
-      <c r="G24" s="170" t="s">
+      <c r="G24" s="169" t="s">
         <v>199</v>
       </c>
       <c r="H24" s="92"/>
@@ -9173,7 +9220,7 @@
     </row>
     <row r="44" spans="1:19" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A44" s="27"/>
-      <c r="B44" s="173" t="s">
+      <c r="B44" s="172" t="s">
         <v>726</v>
       </c>
       <c r="C44" s="115" t="s">
@@ -9319,10 +9366,10 @@
       <c r="B62" s="46"/>
     </row>
     <row r="63" spans="1:10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="167" t="s">
+      <c r="A63" s="166" t="s">
         <v>239</v>
       </c>
-      <c r="B63" s="173"/>
+      <c r="B63" s="172"/>
       <c r="C63" s="115"/>
       <c r="F63" s="110"/>
       <c r="G63" s="28"/>
@@ -9330,7 +9377,7 @@
     </row>
     <row r="64" spans="1:10" ht="34" x14ac:dyDescent="0.15">
       <c r="B64" s="46"/>
-      <c r="C64" s="170" t="s">
+      <c r="C64" s="169" t="s">
         <v>743</v>
       </c>
       <c r="D64" s="26" t="s">
@@ -9612,7 +9659,7 @@
     </row>
     <row r="76" spans="1:10" customFormat="1" ht="34" x14ac:dyDescent="0.15">
       <c r="A76" s="27"/>
-      <c r="B76" s="173" t="s">
+      <c r="B76" s="172" t="s">
         <v>748</v>
       </c>
       <c r="C76" s="115" t="s">

</xml_diff>

<commit_message>
Begin V0.4 firmware branch, monochrome OLED works, working on Unicorn Hat control
</commit_message>
<xml_diff>
--- a/Manufacturing/BOM Core 64 v0.4.0 CB Yellow LB Blue.xlsx
+++ b/Manufacturing/BOM Core 64 v0.4.0 CB Yellow LB Blue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Manufacturing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4725F46F-5F46-4446-AD51-20437620F0F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220C92D1-D7DA-6C43-ADB0-0E3B20DC4679}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="34660" windowHeight="22680" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3077,14 +3077,14 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3582,11 +3582,11 @@
         <v>172</v>
       </c>
       <c r="C3" s="27"/>
-      <c r="P3" s="178" t="s">
+      <c r="P3" s="180" t="s">
         <v>173</v>
       </c>
-      <c r="Q3" s="178"/>
-      <c r="R3" s="178"/>
+      <c r="Q3" s="180"/>
+      <c r="R3" s="180"/>
     </row>
     <row r="4" spans="1:18" ht="51" x14ac:dyDescent="0.15">
       <c r="A4" s="29"/>
@@ -5551,10 +5551,10 @@
   <dimension ref="A1:AF121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="10" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="10" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="B40" sqref="B40"/>
+      <selection pane="bottomRight" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
@@ -5630,11 +5630,11 @@
       <c r="B6" s="92"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="Q7" s="178" t="s">
+      <c r="Q7" s="180" t="s">
         <v>173</v>
       </c>
-      <c r="R7" s="178"/>
-      <c r="S7" s="178"/>
+      <c r="R7" s="180"/>
+      <c r="S7" s="180"/>
     </row>
     <row r="8" spans="1:32" s="83" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A8" s="83" t="s">
@@ -5877,7 +5877,7 @@
     </row>
     <row r="15" spans="1:32" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A15" s="27"/>
-      <c r="B15" s="179" t="s">
+      <c r="B15" s="178" t="s">
         <v>726</v>
       </c>
       <c r="C15" s="115" t="s">
@@ -5927,7 +5927,7 @@
     </row>
     <row r="17" spans="1:9" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A17" s="27"/>
-      <c r="B17" s="179" t="s">
+      <c r="B17" s="178" t="s">
         <v>726</v>
       </c>
       <c r="C17" s="116" t="s">
@@ -5952,7 +5952,7 @@
     </row>
     <row r="18" spans="1:9" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A18" s="27"/>
-      <c r="B18" s="179" t="s">
+      <c r="B18" s="178" t="s">
         <v>726</v>
       </c>
       <c r="C18" s="116" t="s">
@@ -6075,7 +6075,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="23" spans="1:9" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A23" s="27"/>
       <c r="B23" s="172" t="s">
         <v>726</v>
@@ -6103,7 +6103,7 @@
     <row r="24" spans="1:9" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A24" s="27"/>
       <c r="B24" s="172" t="s">
-        <v>726</v>
+        <v>731</v>
       </c>
       <c r="C24" s="115" t="s">
         <v>523</v>
@@ -6221,7 +6221,7 @@
     </row>
     <row r="29" spans="1:9" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A29" s="27"/>
-      <c r="B29" s="180" t="s">
+      <c r="B29" s="179" t="s">
         <v>726</v>
       </c>
       <c r="C29" s="116" t="s">
@@ -6244,7 +6244,7 @@
     </row>
     <row r="30" spans="1:9" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A30" s="27"/>
-      <c r="B30" s="179" t="s">
+      <c r="B30" s="178" t="s">
         <v>726</v>
       </c>
       <c r="C30" s="115" t="s">
@@ -6267,7 +6267,7 @@
     </row>
     <row r="31" spans="1:9" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A31" s="27"/>
-      <c r="B31" s="179" t="s">
+      <c r="B31" s="178" t="s">
         <v>726</v>
       </c>
       <c r="C31" s="116" t="s">
@@ -6313,7 +6313,7 @@
     </row>
     <row r="33" spans="1:19" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A33" s="27"/>
-      <c r="B33" s="179" t="s">
+      <c r="B33" s="178" t="s">
         <v>726</v>
       </c>
       <c r="C33" s="115" t="s">
@@ -6336,7 +6336,7 @@
     </row>
     <row r="34" spans="1:19" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A34" s="27"/>
-      <c r="B34" s="179" t="s">
+      <c r="B34" s="178" t="s">
         <v>726</v>
       </c>
       <c r="C34" s="115" t="s">
@@ -6434,7 +6434,7 @@
     </row>
     <row r="38" spans="1:19" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A38" s="27"/>
-      <c r="B38" s="179" t="s">
+      <c r="B38" s="178" t="s">
         <v>726</v>
       </c>
       <c r="C38" s="115" t="s">
@@ -6459,7 +6459,7 @@
     </row>
     <row r="39" spans="1:19" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A39" s="27"/>
-      <c r="B39" s="179" t="s">
+      <c r="B39" s="178" t="s">
         <v>726</v>
       </c>
       <c r="C39" s="115" t="s">
@@ -8474,11 +8474,11 @@
       <c r="B3" s="29"/>
       <c r="C3" s="27"/>
       <c r="D3" s="27"/>
-      <c r="Q3" s="178" t="s">
+      <c r="Q3" s="180" t="s">
         <v>173</v>
       </c>
-      <c r="R3" s="178"/>
-      <c r="S3" s="178"/>
+      <c r="R3" s="180"/>
+      <c r="S3" s="180"/>
     </row>
     <row r="4" spans="1:19" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" s="29"/>

</xml_diff>

<commit_message>
Add USB and desk stand to BOM
</commit_message>
<xml_diff>
--- a/Manufacturing/BOM Core 64 v0.4.0 CB Yellow LB Blue.xlsx
+++ b/Manufacturing/BOM Core 64 v0.4.0 CB Yellow LB Blue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Manufacturing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA46265A-1953-0141-A174-6D0693D22543}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE46DA08-AA52-5A43-B864-914DFD37DCE9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2480" windowWidth="34660" windowHeight="22680" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2480" windowWidth="34660" windowHeight="22680" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SKU List" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1295" uniqueCount="751">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1300" uniqueCount="756">
   <si>
     <t>Digi-Key Part Number</t>
   </si>
@@ -2307,6 +2307,21 @@
   </si>
   <si>
     <t>Back ordered 329. Change to 303, has much higher inventory.</t>
+  </si>
+  <si>
+    <t>Desk Stand</t>
+  </si>
+  <si>
+    <t>sides, cross bars, screws</t>
+  </si>
+  <si>
+    <t>-OR- Kick-stand</t>
+  </si>
+  <si>
+    <t>USB Cable</t>
+  </si>
+  <si>
+    <t>Programming cable for Teensy</t>
   </si>
 </sst>
 </file>
@@ -2318,10 +2333,24 @@
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -2620,37 +2649,37 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="186">
+  <cellXfs count="189">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="44" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="21" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="20" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="23" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="22" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2660,463 +2689,472 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="18" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="20" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="20" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="20" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="21" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="21" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="4" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="18" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" xfId="4" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="4" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="4" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="19" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="4" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" xfId="4" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="4" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="4" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="20" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3570,7 +3608,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F5DBFB5-E21A-7B4B-815F-748A526FD280}">
   <dimension ref="A1:S68"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
@@ -3618,11 +3656,11 @@
         <v>172</v>
       </c>
       <c r="D3" s="27"/>
-      <c r="Q3" s="182" t="s">
+      <c r="Q3" s="187" t="s">
         <v>173</v>
       </c>
-      <c r="R3" s="182"/>
-      <c r="S3" s="182"/>
+      <c r="R3" s="187"/>
+      <c r="S3" s="187"/>
     </row>
     <row r="4" spans="1:19" ht="51" x14ac:dyDescent="0.15">
       <c r="A4" s="29"/>
@@ -4620,7 +4658,7 @@
       <c r="A29" s="28">
         <v>13</v>
       </c>
-      <c r="B29" s="185" t="s">
+      <c r="B29" s="184" t="s">
         <v>750</v>
       </c>
       <c r="C29" s="47" t="s">
@@ -5605,13 +5643,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1052A41E-3EA7-B148-953B-E2218E71D84C}">
-  <dimension ref="A1:AF121"/>
+  <dimension ref="A1:AF127"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="10" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="10" topLeftCell="B89" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
@@ -5687,11 +5725,11 @@
       <c r="B6" s="92"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="Q7" s="182" t="s">
+      <c r="Q7" s="187" t="s">
         <v>173</v>
       </c>
-      <c r="R7" s="182"/>
-      <c r="S7" s="182"/>
+      <c r="R7" s="187"/>
+      <c r="S7" s="187"/>
     </row>
     <row r="8" spans="1:32" s="83" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A8" s="83" t="s">
@@ -6370,7 +6408,7 @@
     </row>
     <row r="33" spans="1:19" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A33" s="27"/>
-      <c r="B33" s="184" t="s">
+      <c r="B33" s="183" t="s">
         <v>749</v>
       </c>
       <c r="C33" s="115" t="s">
@@ -6393,13 +6431,13 @@
     </row>
     <row r="34" spans="1:19" customFormat="1" ht="17" x14ac:dyDescent="0.15">
       <c r="A34" s="27"/>
-      <c r="B34" s="184" t="s">
+      <c r="B34" s="183" t="s">
         <v>749</v>
       </c>
       <c r="C34" s="115" t="s">
         <v>538</v>
       </c>
-      <c r="D34" s="183">
+      <c r="D34" s="182">
         <v>0.01</v>
       </c>
       <c r="E34" t="s">
@@ -8041,7 +8079,7 @@
     <row r="97" spans="1:19" s="83" customFormat="1" ht="22" x14ac:dyDescent="0.15">
       <c r="B97" s="38"/>
       <c r="C97" s="113" t="s">
-        <v>393</v>
+        <v>751</v>
       </c>
       <c r="D97" s="84"/>
       <c r="E97" s="84"/>
@@ -8057,212 +8095,127 @@
       <c r="R97" s="38"/>
       <c r="S97" s="38"/>
     </row>
-    <row r="98" spans="1:19" s="35" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A98" s="35">
+    <row r="98" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="C98" s="69"/>
+      <c r="D98" s="185" t="s">
+        <v>752</v>
+      </c>
+      <c r="E98" s="69"/>
+    </row>
+    <row r="99" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="C99" s="69"/>
+      <c r="D99" s="186" t="s">
+        <v>753</v>
+      </c>
+      <c r="E99" s="69"/>
+    </row>
+    <row r="100" spans="1:19" s="83" customFormat="1" ht="22" x14ac:dyDescent="0.15">
+      <c r="B100" s="38"/>
+      <c r="C100" s="113" t="s">
+        <v>754</v>
+      </c>
+      <c r="D100" s="84"/>
+      <c r="E100" s="84"/>
+      <c r="F100" s="85"/>
+      <c r="G100" s="57"/>
+      <c r="H100" s="84"/>
+      <c r="I100" s="84"/>
+      <c r="L100" s="38"/>
+      <c r="N100" s="38"/>
+      <c r="O100" s="38"/>
+      <c r="P100" s="38"/>
+      <c r="Q100" s="38"/>
+      <c r="R100" s="38"/>
+      <c r="S100" s="38"/>
+    </row>
+    <row r="101" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="C101" s="69"/>
+      <c r="D101" s="188" t="s">
+        <v>755</v>
+      </c>
+      <c r="E101" s="69"/>
+    </row>
+    <row r="102" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="C102" s="69"/>
+      <c r="D102" s="186"/>
+      <c r="E102" s="69"/>
+    </row>
+    <row r="103" spans="1:19" s="83" customFormat="1" ht="22" x14ac:dyDescent="0.15">
+      <c r="B103" s="38"/>
+      <c r="C103" s="113" t="s">
+        <v>393</v>
+      </c>
+      <c r="D103" s="84"/>
+      <c r="E103" s="84"/>
+      <c r="F103" s="85"/>
+      <c r="G103" s="57"/>
+      <c r="H103" s="84"/>
+      <c r="I103" s="84"/>
+      <c r="L103" s="38"/>
+      <c r="N103" s="38"/>
+      <c r="O103" s="38"/>
+      <c r="P103" s="38"/>
+      <c r="Q103" s="38"/>
+      <c r="R103" s="38"/>
+      <c r="S103" s="38"/>
+    </row>
+    <row r="104" spans="1:19" s="35" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A104" s="35">
         <v>301</v>
       </c>
-      <c r="B98" s="36"/>
-      <c r="C98" s="28" t="s">
+      <c r="B104" s="36"/>
+      <c r="C104" s="28" t="s">
         <v>282</v>
       </c>
-      <c r="E98" s="36" t="s">
+      <c r="E104" s="36" t="s">
         <v>283</v>
       </c>
-      <c r="F98" s="37">
-        <v>1</v>
-      </c>
-      <c r="G98" s="28" t="s">
+      <c r="F104" s="37">
+        <v>1</v>
+      </c>
+      <c r="G104" s="28" t="s">
         <v>198</v>
       </c>
-      <c r="H98" s="36"/>
-      <c r="I98" s="35" t="s">
+      <c r="H104" s="36"/>
+      <c r="I104" s="35" t="s">
         <v>284</v>
       </c>
-      <c r="J98" s="35" t="s">
+      <c r="J104" s="35" t="s">
         <v>201</v>
       </c>
-      <c r="K98" s="35">
-        <v>1</v>
-      </c>
-      <c r="L98" s="35">
-        <f>IF(K98&gt;F98,0,F98-K98)</f>
-        <v>0</v>
-      </c>
-      <c r="M98" s="35">
-        <f>K98+L98</f>
-        <v>1</v>
-      </c>
-      <c r="N98" s="35">
-        <f>M98-F98</f>
-        <v>0</v>
-      </c>
-      <c r="O98" s="35">
-        <f>(4*F98)-N98</f>
+      <c r="K104" s="35">
+        <v>1</v>
+      </c>
+      <c r="L104" s="35">
+        <f>IF(K104&gt;F104,0,F104-K104)</f>
+        <v>0</v>
+      </c>
+      <c r="M104" s="35">
+        <f>K104+L104</f>
+        <v>1</v>
+      </c>
+      <c r="N104" s="35">
+        <f>M104-F104</f>
+        <v>0</v>
+      </c>
+      <c r="O104" s="35">
+        <f>(4*F104)-N104</f>
         <v>4</v>
       </c>
-      <c r="Q98" s="28"/>
-      <c r="R98" s="28"/>
-      <c r="S98" s="28"/>
-    </row>
-    <row r="99" spans="1:19" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A99" s="38">
-        <v>302</v>
-      </c>
-      <c r="C99" s="28" t="s">
-        <v>282</v>
-      </c>
-      <c r="D99" s="35"/>
-      <c r="E99" s="42" t="s">
-        <v>286</v>
-      </c>
-      <c r="F99" s="37">
-        <v>1</v>
-      </c>
-      <c r="G99" s="28" t="s">
-        <v>198</v>
-      </c>
-      <c r="I99" s="83"/>
-      <c r="J99" s="35" t="s">
-        <v>201</v>
-      </c>
-      <c r="S99" s="39"/>
-    </row>
-    <row r="100" spans="1:19" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A100" s="35">
-        <v>303</v>
-      </c>
-      <c r="B100" s="36"/>
-      <c r="C100" s="28" t="s">
-        <v>282</v>
-      </c>
-      <c r="D100" s="35"/>
-      <c r="E100" s="42" t="s">
-        <v>287</v>
-      </c>
-      <c r="F100" s="37">
-        <v>1</v>
-      </c>
-      <c r="G100" s="28" t="s">
-        <v>198</v>
-      </c>
-      <c r="I100" s="83"/>
-      <c r="J100" s="35" t="s">
-        <v>201</v>
-      </c>
-      <c r="S100" s="39"/>
-    </row>
-    <row r="101" spans="1:19" s="97" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A101" s="97">
-        <v>304</v>
-      </c>
-      <c r="C101" s="92" t="s">
-        <v>282</v>
-      </c>
-      <c r="D101" s="98"/>
-      <c r="E101" s="97" t="s">
-        <v>288</v>
-      </c>
-      <c r="F101" s="99">
-        <v>1</v>
-      </c>
-      <c r="G101" s="92" t="s">
-        <v>198</v>
-      </c>
-      <c r="I101" s="94"/>
-      <c r="J101" s="98" t="s">
-        <v>201</v>
-      </c>
-      <c r="S101" s="100"/>
-    </row>
-    <row r="102" spans="1:19" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A102" s="35">
-        <v>305</v>
-      </c>
-      <c r="B102" s="36"/>
-      <c r="C102" s="28" t="s">
-        <v>282</v>
-      </c>
-      <c r="D102" s="35"/>
-      <c r="E102" s="42" t="s">
-        <v>289</v>
-      </c>
-      <c r="F102" s="37">
-        <v>1</v>
-      </c>
-      <c r="G102" s="28" t="s">
-        <v>198</v>
-      </c>
-      <c r="I102" s="83"/>
-      <c r="J102" s="35" t="s">
-        <v>201</v>
-      </c>
-      <c r="K102" s="40"/>
-      <c r="L102" s="40"/>
-      <c r="R102" s="41"/>
-      <c r="S102" s="39"/>
-    </row>
-    <row r="103" spans="1:19" s="97" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A103" s="97">
-        <v>306</v>
-      </c>
-      <c r="C103" s="92" t="s">
-        <v>282</v>
-      </c>
-      <c r="D103" s="98"/>
-      <c r="E103" s="97" t="s">
-        <v>291</v>
-      </c>
-      <c r="F103" s="99">
-        <v>1</v>
-      </c>
-      <c r="G103" s="92" t="s">
-        <v>198</v>
-      </c>
-      <c r="I103" s="94"/>
-      <c r="J103" s="98" t="s">
-        <v>201</v>
-      </c>
-      <c r="K103" s="101"/>
-      <c r="L103" s="101"/>
-      <c r="R103" s="102"/>
-      <c r="S103" s="100"/>
-    </row>
-    <row r="104" spans="1:19" s="97" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A104" s="98">
-        <v>307</v>
-      </c>
-      <c r="B104" s="171"/>
-      <c r="C104" s="92" t="s">
-        <v>282</v>
-      </c>
-      <c r="D104" s="98"/>
-      <c r="E104" s="97" t="s">
-        <v>292</v>
-      </c>
-      <c r="F104" s="99">
-        <v>1</v>
-      </c>
-      <c r="G104" s="92" t="s">
-        <v>198</v>
-      </c>
-      <c r="I104" s="94"/>
-      <c r="J104" s="98" t="s">
-        <v>201</v>
-      </c>
-      <c r="S104" s="100"/>
+      <c r="Q104" s="28"/>
+      <c r="R104" s="28"/>
+      <c r="S104" s="28"/>
     </row>
     <row r="105" spans="1:19" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="38">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="C105" s="28" t="s">
         <v>282</v>
       </c>
-      <c r="D105" s="98" t="s">
-        <v>295</v>
-      </c>
+      <c r="D105" s="35"/>
       <c r="E105" s="42" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="F105" s="37">
         <v>1</v>
@@ -8270,41 +8223,15 @@
       <c r="G105" s="28" t="s">
         <v>198</v>
       </c>
-      <c r="I105" s="120" t="s">
-        <v>295</v>
-      </c>
+      <c r="I105" s="83"/>
       <c r="J105" s="35" t="s">
         <v>201</v>
       </c>
-      <c r="K105" s="38">
-        <v>4</v>
-      </c>
-      <c r="L105" s="38">
-        <v>0</v>
-      </c>
-      <c r="M105" s="35">
-        <f>K105+L105</f>
-        <v>4</v>
-      </c>
-      <c r="N105" s="35">
-        <f>M105-F105</f>
-        <v>3</v>
-      </c>
-      <c r="O105" s="35">
-        <f>(4*F105)-N105</f>
-        <v>1</v>
-      </c>
-      <c r="Q105" s="38">
-        <v>20</v>
-      </c>
-      <c r="R105" s="38">
-        <v>16</v>
-      </c>
       <c r="S105" s="39"/>
     </row>
     <row r="106" spans="1:19" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="35">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="B106" s="36"/>
       <c r="C106" s="28" t="s">
@@ -8312,16 +8239,13 @@
       </c>
       <c r="D106" s="35"/>
       <c r="E106" s="42" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="F106" s="37">
         <v>1</v>
       </c>
       <c r="G106" s="28" t="s">
         <v>198</v>
-      </c>
-      <c r="H106" s="43" t="s">
-        <v>297</v>
       </c>
       <c r="I106" s="83"/>
       <c r="J106" s="35" t="s">
@@ -8329,120 +8253,298 @@
       </c>
       <c r="S106" s="39"/>
     </row>
-    <row r="107" spans="1:19" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A107" s="38">
-        <v>310</v>
-      </c>
-      <c r="C107" s="28" t="s">
+    <row r="107" spans="1:19" s="97" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A107" s="97">
+        <v>304</v>
+      </c>
+      <c r="C107" s="92" t="s">
         <v>282</v>
       </c>
-      <c r="D107" s="35"/>
-      <c r="E107" s="42" t="s">
-        <v>294</v>
-      </c>
-      <c r="F107" s="37">
-        <v>1</v>
-      </c>
-      <c r="G107" s="28" t="s">
+      <c r="D107" s="98"/>
+      <c r="E107" s="97" t="s">
+        <v>288</v>
+      </c>
+      <c r="F107" s="99">
+        <v>1</v>
+      </c>
+      <c r="G107" s="92" t="s">
         <v>198</v>
       </c>
-      <c r="H107" s="43" t="s">
-        <v>297</v>
-      </c>
-      <c r="I107" s="83"/>
-      <c r="J107" s="35" t="s">
+      <c r="I107" s="94"/>
+      <c r="J107" s="98" t="s">
         <v>201</v>
       </c>
-      <c r="S107" s="39"/>
+      <c r="S107" s="100"/>
     </row>
     <row r="108" spans="1:19" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A108" s="38">
-        <v>311</v>
-      </c>
+      <c r="A108" s="35">
+        <v>305</v>
+      </c>
+      <c r="B108" s="36"/>
       <c r="C108" s="28" t="s">
         <v>282</v>
       </c>
       <c r="D108" s="35"/>
-      <c r="E108" s="43" t="s">
+      <c r="E108" s="42" t="s">
+        <v>289</v>
+      </c>
+      <c r="F108" s="37">
+        <v>1</v>
+      </c>
+      <c r="G108" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="I108" s="83"/>
+      <c r="J108" s="35" t="s">
+        <v>201</v>
+      </c>
+      <c r="K108" s="40"/>
+      <c r="L108" s="40"/>
+      <c r="R108" s="41"/>
+      <c r="S108" s="39"/>
+    </row>
+    <row r="109" spans="1:19" s="97" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A109" s="97">
+        <v>306</v>
+      </c>
+      <c r="C109" s="92" t="s">
+        <v>282</v>
+      </c>
+      <c r="D109" s="98"/>
+      <c r="E109" s="97" t="s">
+        <v>291</v>
+      </c>
+      <c r="F109" s="99">
+        <v>1</v>
+      </c>
+      <c r="G109" s="92" t="s">
+        <v>198</v>
+      </c>
+      <c r="I109" s="94"/>
+      <c r="J109" s="98" t="s">
+        <v>201</v>
+      </c>
+      <c r="K109" s="101"/>
+      <c r="L109" s="101"/>
+      <c r="R109" s="102"/>
+      <c r="S109" s="100"/>
+    </row>
+    <row r="110" spans="1:19" s="97" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A110" s="98">
+        <v>307</v>
+      </c>
+      <c r="B110" s="171"/>
+      <c r="C110" s="92" t="s">
+        <v>282</v>
+      </c>
+      <c r="D110" s="98"/>
+      <c r="E110" s="97" t="s">
+        <v>292</v>
+      </c>
+      <c r="F110" s="99">
+        <v>1</v>
+      </c>
+      <c r="G110" s="92" t="s">
+        <v>198</v>
+      </c>
+      <c r="I110" s="94"/>
+      <c r="J110" s="98" t="s">
+        <v>201</v>
+      </c>
+      <c r="S110" s="100"/>
+    </row>
+    <row r="111" spans="1:19" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A111" s="38">
+        <v>308</v>
+      </c>
+      <c r="C111" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="D111" s="98" t="s">
+        <v>295</v>
+      </c>
+      <c r="E111" s="42" t="s">
+        <v>290</v>
+      </c>
+      <c r="F111" s="37">
+        <v>1</v>
+      </c>
+      <c r="G111" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="I111" s="120" t="s">
+        <v>295</v>
+      </c>
+      <c r="J111" s="35" t="s">
+        <v>201</v>
+      </c>
+      <c r="K111" s="38">
+        <v>4</v>
+      </c>
+      <c r="L111" s="38">
+        <v>0</v>
+      </c>
+      <c r="M111" s="35">
+        <f>K111+L111</f>
+        <v>4</v>
+      </c>
+      <c r="N111" s="35">
+        <f>M111-F111</f>
+        <v>3</v>
+      </c>
+      <c r="O111" s="35">
+        <f>(4*F111)-N111</f>
+        <v>1</v>
+      </c>
+      <c r="Q111" s="38">
+        <v>20</v>
+      </c>
+      <c r="R111" s="38">
+        <v>16</v>
+      </c>
+      <c r="S111" s="39"/>
+    </row>
+    <row r="112" spans="1:19" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A112" s="35">
+        <v>309</v>
+      </c>
+      <c r="B112" s="36"/>
+      <c r="C112" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="D112" s="35"/>
+      <c r="E112" s="42" t="s">
+        <v>293</v>
+      </c>
+      <c r="F112" s="37">
+        <v>1</v>
+      </c>
+      <c r="G112" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="H112" s="43" t="s">
+        <v>297</v>
+      </c>
+      <c r="I112" s="83"/>
+      <c r="J112" s="35" t="s">
+        <v>201</v>
+      </c>
+      <c r="S112" s="39"/>
+    </row>
+    <row r="113" spans="1:19" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A113" s="38">
+        <v>310</v>
+      </c>
+      <c r="C113" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="D113" s="35"/>
+      <c r="E113" s="42" t="s">
+        <v>294</v>
+      </c>
+      <c r="F113" s="37">
+        <v>1</v>
+      </c>
+      <c r="G113" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="H113" s="43" t="s">
+        <v>297</v>
+      </c>
+      <c r="I113" s="83"/>
+      <c r="J113" s="35" t="s">
+        <v>201</v>
+      </c>
+      <c r="S113" s="39"/>
+    </row>
+    <row r="114" spans="1:19" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A114" s="38">
+        <v>311</v>
+      </c>
+      <c r="C114" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="D114" s="35"/>
+      <c r="E114" s="43" t="s">
         <v>296</v>
       </c>
-      <c r="F108" s="86"/>
-      <c r="H108" s="43" t="s">
+      <c r="F114" s="86"/>
+      <c r="H114" s="43" t="s">
         <v>298</v>
       </c>
-      <c r="I108" s="83"/>
-      <c r="J108" s="43" t="s">
+      <c r="I114" s="83"/>
+      <c r="J114" s="43" t="s">
         <v>201</v>
       </c>
-      <c r="S108" s="39"/>
-    </row>
-    <row r="109" spans="1:19" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A109" s="38">
+      <c r="S114" s="39"/>
+    </row>
+    <row r="115" spans="1:19" s="38" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A115" s="38">
         <v>312</v>
       </c>
-      <c r="C109" s="28" t="s">
+      <c r="C115" s="28" t="s">
         <v>282</v>
       </c>
-      <c r="D109" s="35"/>
-      <c r="E109" s="43" t="s">
+      <c r="D115" s="35"/>
+      <c r="E115" s="43" t="s">
         <v>299</v>
       </c>
-      <c r="F109" s="37">
-        <v>1</v>
-      </c>
-      <c r="G109" s="43" t="s">
+      <c r="F115" s="37">
+        <v>1</v>
+      </c>
+      <c r="G115" s="43" t="s">
         <v>198</v>
       </c>
-      <c r="H109" s="43" t="s">
+      <c r="H115" s="43" t="s">
         <v>300</v>
       </c>
-      <c r="I109" s="83"/>
-      <c r="J109" s="43" t="s">
+      <c r="I115" s="83"/>
+      <c r="J115" s="43" t="s">
         <v>201</v>
       </c>
-      <c r="S109" s="39"/>
-    </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="C110" s="28"/>
-    </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="C111" s="28"/>
-    </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="C112" s="28"/>
-    </row>
-    <row r="113" spans="3:3" x14ac:dyDescent="0.15">
-      <c r="C113" s="28"/>
-    </row>
-    <row r="114" spans="3:3" x14ac:dyDescent="0.15">
-      <c r="C114" s="28"/>
-    </row>
-    <row r="115" spans="3:3" x14ac:dyDescent="0.15">
-      <c r="C115" s="28"/>
-    </row>
-    <row r="116" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="S115" s="39"/>
+    </row>
+    <row r="116" spans="1:19" x14ac:dyDescent="0.15">
       <c r="C116" s="28"/>
     </row>
-    <row r="117" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:19" x14ac:dyDescent="0.15">
       <c r="C117" s="28"/>
     </row>
-    <row r="118" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:19" x14ac:dyDescent="0.15">
       <c r="C118" s="28"/>
     </row>
-    <row r="119" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:19" x14ac:dyDescent="0.15">
       <c r="C119" s="28"/>
     </row>
-    <row r="120" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:19" x14ac:dyDescent="0.15">
       <c r="C120" s="28"/>
     </row>
-    <row r="121" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:19" x14ac:dyDescent="0.15">
       <c r="C121" s="28"/>
+    </row>
+    <row r="122" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="C122" s="28"/>
+    </row>
+    <row r="123" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="C123" s="28"/>
+    </row>
+    <row r="124" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="C124" s="28"/>
+    </row>
+    <row r="125" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="C125" s="28"/>
+    </row>
+    <row r="126" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="C126" s="28"/>
+    </row>
+    <row r="127" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="C127" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="Q7:S7"/>
   </mergeCells>
-  <phoneticPr fontId="23" type="noConversion"/>
+  <phoneticPr fontId="25" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="I21" r:id="rId1" xr:uid="{B3564F39-BDFC-024B-80FC-3B84D3B19B84}"/>
     <hyperlink ref="I19" r:id="rId2" xr:uid="{441A81FD-7638-214B-A580-55099579328C}"/>
@@ -8494,7 +8596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6340416-D374-C841-832D-DB1142BA15CE}">
   <dimension ref="A1:S77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="125" workbookViewId="0">
+    <sheetView topLeftCell="A46" zoomScale="125" workbookViewId="0">
       <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
@@ -8532,11 +8634,11 @@
       <c r="B3" s="29"/>
       <c r="C3" s="27"/>
       <c r="D3" s="27"/>
-      <c r="Q3" s="182" t="s">
+      <c r="Q3" s="187" t="s">
         <v>173</v>
       </c>
-      <c r="R3" s="182"/>
-      <c r="S3" s="182"/>
+      <c r="R3" s="187"/>
+      <c r="S3" s="187"/>
     </row>
     <row r="4" spans="1:19" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" s="29"/>

</xml_diff>